<commit_message>
Added 'AudioFiltering' and 'Codec' sheets to PCB schematic, started PCB layout with decouple caps and MCU. The codec in sheet 'Codec' is wrong, placed for testing
</commit_message>
<xml_diff>
--- a/Super Epische Audio Generator/Seminaries/planning_audio_generator.xlsx
+++ b/Super Epische Audio Generator/Seminaries/planning_audio_generator.xlsx
@@ -2328,8 +2328,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BP49"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" showRuler="0" topLeftCell="A11" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView showGridLines="0" tabSelected="1" showRuler="0" topLeftCell="A29" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
+      <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2493,7 +2493,7 @@
       </c>
       <c r="C6" s="33" cm="1">
         <f t="array" aca="1" ref="C6" ca="1">IFERROR(IF(MIN(Milestones4352[Start])=0,TODAY(),B11(Milestones4352[Start])),TODAY())</f>
-        <v>45351</v>
+        <v>45356</v>
       </c>
       <c r="D6" s="34"/>
       <c r="E6" s="28"/>
@@ -2502,7 +2502,7 @@
       <c r="H6" s="28"/>
       <c r="I6" s="44" t="str">
         <f ca="1">TEXT(I7,"mmmm")</f>
-        <v>February</v>
+        <v>March</v>
       </c>
       <c r="J6" s="44"/>
       <c r="K6" s="44"/>
@@ -2512,7 +2512,7 @@
       <c r="O6" s="44"/>
       <c r="P6" s="44" t="str">
         <f ca="1">IF(TEXT(P7,"mmmm")=I6,"",TEXT(P7,"mmmm"))</f>
-        <v>March</v>
+        <v/>
       </c>
       <c r="Q6" s="44"/>
       <c r="R6" s="44"/>
@@ -2542,7 +2542,7 @@
       <c r="AJ6" s="44"/>
       <c r="AK6" s="44" t="str">
         <f ca="1">IF(OR(TEXT(AK7,"mmmm")=AD6,TEXT(AK7,"mmmm")=W6,TEXT(AK7,"mmmm")=P6,TEXT(AK7,"mmmm")=I6),"",TEXT(AK7,"mmmm"))</f>
-        <v/>
+        <v>April</v>
       </c>
       <c r="AL6" s="44"/>
       <c r="AM6" s="44"/>
@@ -2552,7 +2552,7 @@
       <c r="AQ6" s="44"/>
       <c r="AR6" s="44" t="str">
         <f ca="1">IF(OR(TEXT(AR7,"mmmm")=AK6,TEXT(AR7,"mmmm")=AD6,TEXT(AR7,"mmmm")=W6,TEXT(AR7,"mmmm")=P6),"",TEXT(AR7,"mmmm"))</f>
-        <v>April</v>
+        <v/>
       </c>
       <c r="AS6" s="44"/>
       <c r="AT6" s="44"/>
@@ -2596,227 +2596,227 @@
       <c r="H7" s="36"/>
       <c r="I7" s="51">
         <f ca="1">IFERROR(Project_Start+Scrolverhoging,TODAY())</f>
-        <v>45351</v>
+        <v>45356</v>
       </c>
       <c r="J7" s="52">
         <f ca="1">I7+1</f>
-        <v>45352</v>
+        <v>45357</v>
       </c>
       <c r="K7" s="52">
         <f t="shared" ref="K7:AX7" ca="1" si="0">J7+1</f>
-        <v>45353</v>
+        <v>45358</v>
       </c>
       <c r="L7" s="52">
         <f t="shared" ca="1" si="0"/>
-        <v>45354</v>
+        <v>45359</v>
       </c>
       <c r="M7" s="52">
         <f t="shared" ca="1" si="0"/>
-        <v>45355</v>
+        <v>45360</v>
       </c>
       <c r="N7" s="52">
         <f t="shared" ca="1" si="0"/>
-        <v>45356</v>
+        <v>45361</v>
       </c>
       <c r="O7" s="53">
         <f t="shared" ca="1" si="0"/>
-        <v>45357</v>
+        <v>45362</v>
       </c>
       <c r="P7" s="52">
         <f ca="1">O7+1</f>
-        <v>45358</v>
+        <v>45363</v>
       </c>
       <c r="Q7" s="52">
         <f ca="1">P7+1</f>
-        <v>45359</v>
+        <v>45364</v>
       </c>
       <c r="R7" s="52">
         <f t="shared" ca="1" si="0"/>
-        <v>45360</v>
+        <v>45365</v>
       </c>
       <c r="S7" s="52">
         <f t="shared" ca="1" si="0"/>
-        <v>45361</v>
+        <v>45366</v>
       </c>
       <c r="T7" s="52">
         <f t="shared" ca="1" si="0"/>
-        <v>45362</v>
+        <v>45367</v>
       </c>
       <c r="U7" s="52">
         <f t="shared" ca="1" si="0"/>
-        <v>45363</v>
+        <v>45368</v>
       </c>
       <c r="V7" s="53">
         <f t="shared" ca="1" si="0"/>
-        <v>45364</v>
+        <v>45369</v>
       </c>
       <c r="W7" s="52">
         <f ca="1">V7+1</f>
-        <v>45365</v>
+        <v>45370</v>
       </c>
       <c r="X7" s="52">
         <f ca="1">W7+1</f>
-        <v>45366</v>
+        <v>45371</v>
       </c>
       <c r="Y7" s="52">
         <f t="shared" ca="1" si="0"/>
-        <v>45367</v>
+        <v>45372</v>
       </c>
       <c r="Z7" s="52">
         <f t="shared" ca="1" si="0"/>
-        <v>45368</v>
+        <v>45373</v>
       </c>
       <c r="AA7" s="52">
         <f t="shared" ca="1" si="0"/>
-        <v>45369</v>
+        <v>45374</v>
       </c>
       <c r="AB7" s="52">
         <f t="shared" ca="1" si="0"/>
-        <v>45370</v>
+        <v>45375</v>
       </c>
       <c r="AC7" s="53">
         <f t="shared" ca="1" si="0"/>
-        <v>45371</v>
+        <v>45376</v>
       </c>
       <c r="AD7" s="52">
         <f ca="1">AC7+1</f>
-        <v>45372</v>
+        <v>45377</v>
       </c>
       <c r="AE7" s="52">
         <f ca="1">AD7+1</f>
-        <v>45373</v>
+        <v>45378</v>
       </c>
       <c r="AF7" s="52">
         <f t="shared" ca="1" si="0"/>
-        <v>45374</v>
+        <v>45379</v>
       </c>
       <c r="AG7" s="52">
         <f t="shared" ca="1" si="0"/>
-        <v>45375</v>
+        <v>45380</v>
       </c>
       <c r="AH7" s="52">
         <f t="shared" ca="1" si="0"/>
-        <v>45376</v>
+        <v>45381</v>
       </c>
       <c r="AI7" s="52">
         <f t="shared" ca="1" si="0"/>
-        <v>45377</v>
+        <v>45382</v>
       </c>
       <c r="AJ7" s="53">
         <f t="shared" ca="1" si="0"/>
-        <v>45378</v>
+        <v>45383</v>
       </c>
       <c r="AK7" s="52">
         <f ca="1">AJ7+1</f>
-        <v>45379</v>
+        <v>45384</v>
       </c>
       <c r="AL7" s="52">
         <f ca="1">AK7+1</f>
-        <v>45380</v>
+        <v>45385</v>
       </c>
       <c r="AM7" s="52">
         <f t="shared" ca="1" si="0"/>
-        <v>45381</v>
+        <v>45386</v>
       </c>
       <c r="AN7" s="52">
         <f t="shared" ca="1" si="0"/>
-        <v>45382</v>
+        <v>45387</v>
       </c>
       <c r="AO7" s="52">
         <f t="shared" ca="1" si="0"/>
-        <v>45383</v>
+        <v>45388</v>
       </c>
       <c r="AP7" s="52">
         <f t="shared" ca="1" si="0"/>
-        <v>45384</v>
+        <v>45389</v>
       </c>
       <c r="AQ7" s="53">
         <f t="shared" ca="1" si="0"/>
-        <v>45385</v>
+        <v>45390</v>
       </c>
       <c r="AR7" s="52">
         <f ca="1">AQ7+1</f>
-        <v>45386</v>
+        <v>45391</v>
       </c>
       <c r="AS7" s="52">
         <f ca="1">AR7+1</f>
-        <v>45387</v>
+        <v>45392</v>
       </c>
       <c r="AT7" s="52">
         <f t="shared" ca="1" si="0"/>
-        <v>45388</v>
+        <v>45393</v>
       </c>
       <c r="AU7" s="52">
         <f t="shared" ca="1" si="0"/>
-        <v>45389</v>
+        <v>45394</v>
       </c>
       <c r="AV7" s="52">
         <f t="shared" ca="1" si="0"/>
-        <v>45390</v>
+        <v>45395</v>
       </c>
       <c r="AW7" s="52">
         <f t="shared" ca="1" si="0"/>
-        <v>45391</v>
+        <v>45396</v>
       </c>
       <c r="AX7" s="53">
         <f t="shared" ca="1" si="0"/>
-        <v>45392</v>
+        <v>45397</v>
       </c>
       <c r="AY7" s="52">
         <f ca="1">AX7+1</f>
-        <v>45393</v>
+        <v>45398</v>
       </c>
       <c r="AZ7" s="52">
         <f ca="1">AY7+1</f>
-        <v>45394</v>
+        <v>45399</v>
       </c>
       <c r="BA7" s="52">
         <f t="shared" ref="BA7:BE7" ca="1" si="1">AZ7+1</f>
-        <v>45395</v>
+        <v>45400</v>
       </c>
       <c r="BB7" s="52">
         <f t="shared" ca="1" si="1"/>
-        <v>45396</v>
+        <v>45401</v>
       </c>
       <c r="BC7" s="52">
         <f t="shared" ca="1" si="1"/>
-        <v>45397</v>
+        <v>45402</v>
       </c>
       <c r="BD7" s="52">
         <f t="shared" ca="1" si="1"/>
-        <v>45398</v>
+        <v>45403</v>
       </c>
       <c r="BE7" s="53">
         <f t="shared" ca="1" si="1"/>
-        <v>45399</v>
+        <v>45404</v>
       </c>
       <c r="BF7" s="52">
         <f ca="1">BE7+1</f>
-        <v>45400</v>
+        <v>45405</v>
       </c>
       <c r="BG7" s="52">
         <f ca="1">BF7+1</f>
-        <v>45401</v>
+        <v>45406</v>
       </c>
       <c r="BH7" s="52">
         <f t="shared" ref="BH7:BL7" ca="1" si="2">BG7+1</f>
-        <v>45402</v>
+        <v>45407</v>
       </c>
       <c r="BI7" s="52">
         <f t="shared" ca="1" si="2"/>
-        <v>45403</v>
+        <v>45408</v>
       </c>
       <c r="BJ7" s="52">
         <f t="shared" ca="1" si="2"/>
-        <v>45404</v>
+        <v>45409</v>
       </c>
       <c r="BK7" s="52">
         <f t="shared" ca="1" si="2"/>
-        <v>45405</v>
+        <v>45410</v>
       </c>
       <c r="BL7" s="53">
         <f t="shared" ca="1" si="2"/>
-        <v>45406</v>
+        <v>45411</v>
       </c>
     </row>
     <row r="8" spans="1:68" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
@@ -2912,27 +2912,27 @@
       </c>
       <c r="J9" s="47" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>F</v>
+        <v>W</v>
       </c>
       <c r="K9" s="47" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>S</v>
+        <v>T</v>
       </c>
       <c r="L9" s="47" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>S</v>
+        <v>F</v>
       </c>
       <c r="M9" s="47" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>M</v>
+        <v>S</v>
       </c>
       <c r="N9" s="47" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>T</v>
+        <v>S</v>
       </c>
       <c r="O9" s="47" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>W</v>
+        <v>M</v>
       </c>
       <c r="P9" s="47" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -2940,27 +2940,27 @@
       </c>
       <c r="Q9" s="47" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>F</v>
+        <v>W</v>
       </c>
       <c r="R9" s="47" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>S</v>
+        <v>T</v>
       </c>
       <c r="S9" s="47" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>S</v>
+        <v>F</v>
       </c>
       <c r="T9" s="47" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>M</v>
+        <v>S</v>
       </c>
       <c r="U9" s="47" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>T</v>
+        <v>S</v>
       </c>
       <c r="V9" s="47" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>W</v>
+        <v>M</v>
       </c>
       <c r="W9" s="47" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -2968,27 +2968,27 @@
       </c>
       <c r="X9" s="47" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>F</v>
+        <v>W</v>
       </c>
       <c r="Y9" s="47" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>S</v>
+        <v>T</v>
       </c>
       <c r="Z9" s="47" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>S</v>
+        <v>F</v>
       </c>
       <c r="AA9" s="47" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>M</v>
+        <v>S</v>
       </c>
       <c r="AB9" s="47" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>T</v>
+        <v>S</v>
       </c>
       <c r="AC9" s="47" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>W</v>
+        <v>M</v>
       </c>
       <c r="AD9" s="47" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -2996,27 +2996,27 @@
       </c>
       <c r="AE9" s="47" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>F</v>
+        <v>W</v>
       </c>
       <c r="AF9" s="47" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>S</v>
+        <v>T</v>
       </c>
       <c r="AG9" s="47" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>S</v>
+        <v>F</v>
       </c>
       <c r="AH9" s="47" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>M</v>
+        <v>S</v>
       </c>
       <c r="AI9" s="47" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>T</v>
+        <v>S</v>
       </c>
       <c r="AJ9" s="47" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>W</v>
+        <v>M</v>
       </c>
       <c r="AK9" s="47" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -3024,27 +3024,27 @@
       </c>
       <c r="AL9" s="47" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>F</v>
+        <v>W</v>
       </c>
       <c r="AM9" s="47" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>S</v>
+        <v>T</v>
       </c>
       <c r="AN9" s="47" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>S</v>
+        <v>F</v>
       </c>
       <c r="AO9" s="47" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>M</v>
+        <v>S</v>
       </c>
       <c r="AP9" s="47" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>T</v>
+        <v>S</v>
       </c>
       <c r="AQ9" s="47" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>W</v>
+        <v>M</v>
       </c>
       <c r="AR9" s="47" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -3052,27 +3052,27 @@
       </c>
       <c r="AS9" s="47" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>F</v>
+        <v>W</v>
       </c>
       <c r="AT9" s="47" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>S</v>
+        <v>T</v>
       </c>
       <c r="AU9" s="47" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>S</v>
+        <v>F</v>
       </c>
       <c r="AV9" s="47" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>M</v>
+        <v>S</v>
       </c>
       <c r="AW9" s="47" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>T</v>
+        <v>S</v>
       </c>
       <c r="AX9" s="47" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>W</v>
+        <v>M</v>
       </c>
       <c r="AY9" s="47" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -3080,27 +3080,27 @@
       </c>
       <c r="AZ9" s="47" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>F</v>
+        <v>W</v>
       </c>
       <c r="BA9" s="47" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>S</v>
+        <v>T</v>
       </c>
       <c r="BB9" s="47" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>S</v>
+        <v>F</v>
       </c>
       <c r="BC9" s="47" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>M</v>
+        <v>S</v>
       </c>
       <c r="BD9" s="47" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>T</v>
+        <v>S</v>
       </c>
       <c r="BE9" s="47" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>W</v>
+        <v>M</v>
       </c>
       <c r="BF9" s="47" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -3108,27 +3108,27 @@
       </c>
       <c r="BG9" s="47" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>F</v>
+        <v>W</v>
       </c>
       <c r="BH9" s="47" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>S</v>
+        <v>T</v>
       </c>
       <c r="BI9" s="47" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>S</v>
+        <v>F</v>
       </c>
       <c r="BJ9" s="47" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>M</v>
+        <v>S</v>
       </c>
       <c r="BK9" s="47" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>T</v>
+        <v>S</v>
       </c>
       <c r="BL9" s="47" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>W</v>
+        <v>M</v>
       </c>
     </row>
     <row r="10" spans="1:68" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
@@ -3446,7 +3446,7 @@
       </c>
       <c r="F12" s="17">
         <f ca="1">TODAY()</f>
-        <v>45351</v>
+        <v>45356</v>
       </c>
       <c r="G12" s="18">
         <v>11</v>
@@ -3802,25 +3802,25 @@
         <f t="shared" ca="1" si="5"/>
         <v/>
       </c>
-      <c r="AJ13" s="12" t="str">
+      <c r="AJ13" s="12">
         <f t="shared" ca="1" si="5"/>
-        <v/>
-      </c>
-      <c r="AK13" s="12" t="str">
+        <v>2</v>
+      </c>
+      <c r="AK13" s="12">
         <f t="shared" ca="1" si="5"/>
-        <v/>
-      </c>
-      <c r="AL13" s="12" t="str">
+        <v>2</v>
+      </c>
+      <c r="AL13" s="12">
         <f t="shared" ca="1" si="5"/>
-        <v/>
-      </c>
-      <c r="AM13" s="12" t="str">
+        <v>2</v>
+      </c>
+      <c r="AM13" s="12">
         <f t="shared" ca="1" si="5"/>
-        <v/>
-      </c>
-      <c r="AN13" s="12" t="str">
+        <v>2</v>
+      </c>
+      <c r="AN13" s="12">
         <f t="shared" ca="1" si="5"/>
-        <v/>
+        <v>2</v>
       </c>
       <c r="AO13" s="12">
         <f t="shared" ca="1" si="6"/>
@@ -3858,25 +3858,25 @@
         <f t="shared" ca="1" si="6"/>
         <v>2</v>
       </c>
-      <c r="AX13" s="12">
+      <c r="AX13" s="12" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>2</v>
-      </c>
-      <c r="AY13" s="12">
+        <v/>
+      </c>
+      <c r="AY13" s="12" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>2</v>
-      </c>
-      <c r="AZ13" s="12">
+        <v/>
+      </c>
+      <c r="AZ13" s="12" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>2</v>
-      </c>
-      <c r="BA13" s="12">
+        <v/>
+      </c>
+      <c r="BA13" s="12" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>2</v>
-      </c>
-      <c r="BB13" s="12">
+        <v/>
+      </c>
+      <c r="BB13" s="12" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>2</v>
+        <v/>
       </c>
       <c r="BC13" s="12" t="str">
         <f t="shared" ca="1" si="6"/>
@@ -4044,25 +4044,25 @@
         <f t="shared" ca="1" si="11"/>
         <v/>
       </c>
-      <c r="AJ14" s="12" t="str">
+      <c r="AJ14" s="12">
         <f t="shared" ca="1" si="11"/>
-        <v/>
-      </c>
-      <c r="AK14" s="12" t="str">
+        <v>2</v>
+      </c>
+      <c r="AK14" s="12">
         <f t="shared" ca="1" si="11"/>
-        <v/>
-      </c>
-      <c r="AL14" s="12" t="str">
+        <v>2</v>
+      </c>
+      <c r="AL14" s="12">
         <f t="shared" ca="1" si="11"/>
-        <v/>
-      </c>
-      <c r="AM14" s="12" t="str">
+        <v>2</v>
+      </c>
+      <c r="AM14" s="12">
         <f t="shared" ref="AM14:AV23" ca="1" si="12">IF(AND($C14="Doel",AM$7&gt;=$F14,AM$7&lt;=$F14+$G14-1),2,IF(AND($C14="Mijlpaal",AM$7&gt;=$F14,AM$7&lt;=$F14+$G14-1),1,""))</f>
-        <v/>
-      </c>
-      <c r="AN14" s="12" t="str">
+        <v>2</v>
+      </c>
+      <c r="AN14" s="12">
         <f t="shared" ca="1" si="12"/>
-        <v/>
+        <v>2</v>
       </c>
       <c r="AO14" s="12">
         <f t="shared" ca="1" si="12"/>
@@ -4100,25 +4100,25 @@
         <f t="shared" ref="AW14:BF23" ca="1" si="13">IF(AND($C14="Doel",AW$7&gt;=$F14,AW$7&lt;=$F14+$G14-1),2,IF(AND($C14="Mijlpaal",AW$7&gt;=$F14,AW$7&lt;=$F14+$G14-1),1,""))</f>
         <v>2</v>
       </c>
-      <c r="AX14" s="12">
+      <c r="AX14" s="12" t="str">
         <f t="shared" ca="1" si="13"/>
-        <v>2</v>
-      </c>
-      <c r="AY14" s="12">
+        <v/>
+      </c>
+      <c r="AY14" s="12" t="str">
         <f t="shared" ca="1" si="13"/>
-        <v>2</v>
-      </c>
-      <c r="AZ14" s="12">
+        <v/>
+      </c>
+      <c r="AZ14" s="12" t="str">
         <f t="shared" ca="1" si="13"/>
-        <v>2</v>
-      </c>
-      <c r="BA14" s="12">
+        <v/>
+      </c>
+      <c r="BA14" s="12" t="str">
         <f t="shared" ca="1" si="13"/>
-        <v>2</v>
-      </c>
-      <c r="BB14" s="12">
+        <v/>
+      </c>
+      <c r="BB14" s="12" t="str">
         <f t="shared" ca="1" si="13"/>
-        <v>2</v>
+        <v/>
       </c>
       <c r="BC14" s="12" t="str">
         <f t="shared" ca="1" si="13"/>
@@ -4286,25 +4286,25 @@
         <f t="shared" ca="1" si="11"/>
         <v/>
       </c>
-      <c r="AJ15" s="12" t="str">
+      <c r="AJ15" s="12">
         <f t="shared" ca="1" si="11"/>
-        <v/>
-      </c>
-      <c r="AK15" s="12" t="str">
+        <v>2</v>
+      </c>
+      <c r="AK15" s="12">
         <f t="shared" ca="1" si="11"/>
-        <v/>
-      </c>
-      <c r="AL15" s="12" t="str">
+        <v>2</v>
+      </c>
+      <c r="AL15" s="12">
         <f t="shared" ca="1" si="11"/>
-        <v/>
-      </c>
-      <c r="AM15" s="12" t="str">
+        <v>2</v>
+      </c>
+      <c r="AM15" s="12">
         <f t="shared" ca="1" si="12"/>
-        <v/>
-      </c>
-      <c r="AN15" s="12" t="str">
+        <v>2</v>
+      </c>
+      <c r="AN15" s="12">
         <f t="shared" ca="1" si="12"/>
-        <v/>
+        <v>2</v>
       </c>
       <c r="AO15" s="12">
         <f t="shared" ca="1" si="12"/>
@@ -4342,25 +4342,25 @@
         <f t="shared" ca="1" si="13"/>
         <v>2</v>
       </c>
-      <c r="AX15" s="12">
+      <c r="AX15" s="12" t="str">
         <f t="shared" ca="1" si="13"/>
-        <v>2</v>
-      </c>
-      <c r="AY15" s="12">
+        <v/>
+      </c>
+      <c r="AY15" s="12" t="str">
         <f t="shared" ca="1" si="13"/>
-        <v>2</v>
-      </c>
-      <c r="AZ15" s="12">
+        <v/>
+      </c>
+      <c r="AZ15" s="12" t="str">
         <f t="shared" ca="1" si="13"/>
-        <v>2</v>
-      </c>
-      <c r="BA15" s="12">
+        <v/>
+      </c>
+      <c r="BA15" s="12" t="str">
         <f t="shared" ca="1" si="13"/>
-        <v>2</v>
-      </c>
-      <c r="BB15" s="12">
+        <v/>
+      </c>
+      <c r="BB15" s="12" t="str">
         <f t="shared" ca="1" si="13"/>
-        <v>2</v>
+        <v/>
       </c>
       <c r="BC15" s="12" t="str">
         <f t="shared" ca="1" si="13"/>
@@ -4528,25 +4528,25 @@
         <f t="shared" ca="1" si="11"/>
         <v/>
       </c>
-      <c r="AJ16" s="12" t="str">
+      <c r="AJ16" s="12">
         <f t="shared" ca="1" si="11"/>
-        <v/>
-      </c>
-      <c r="AK16" s="12" t="str">
+        <v>2</v>
+      </c>
+      <c r="AK16" s="12">
         <f t="shared" ca="1" si="11"/>
-        <v/>
-      </c>
-      <c r="AL16" s="12" t="str">
+        <v>2</v>
+      </c>
+      <c r="AL16" s="12">
         <f t="shared" ca="1" si="11"/>
-        <v/>
-      </c>
-      <c r="AM16" s="12" t="str">
+        <v>2</v>
+      </c>
+      <c r="AM16" s="12">
         <f t="shared" ca="1" si="12"/>
-        <v/>
-      </c>
-      <c r="AN16" s="12" t="str">
+        <v>2</v>
+      </c>
+      <c r="AN16" s="12">
         <f t="shared" ca="1" si="12"/>
-        <v/>
+        <v>2</v>
       </c>
       <c r="AO16" s="12">
         <f t="shared" ca="1" si="12"/>
@@ -4556,25 +4556,25 @@
         <f t="shared" ca="1" si="12"/>
         <v>2</v>
       </c>
-      <c r="AQ16" s="12">
+      <c r="AQ16" s="12" t="str">
         <f t="shared" ca="1" si="12"/>
-        <v>2</v>
-      </c>
-      <c r="AR16" s="12">
+        <v/>
+      </c>
+      <c r="AR16" s="12" t="str">
         <f t="shared" ca="1" si="12"/>
-        <v>2</v>
-      </c>
-      <c r="AS16" s="12">
+        <v/>
+      </c>
+      <c r="AS16" s="12" t="str">
         <f t="shared" ca="1" si="12"/>
-        <v>2</v>
-      </c>
-      <c r="AT16" s="12">
+        <v/>
+      </c>
+      <c r="AT16" s="12" t="str">
         <f t="shared" ca="1" si="12"/>
-        <v>2</v>
-      </c>
-      <c r="AU16" s="12">
+        <v/>
+      </c>
+      <c r="AU16" s="12" t="str">
         <f t="shared" ca="1" si="12"/>
-        <v>2</v>
+        <v/>
       </c>
       <c r="AV16" s="12" t="str">
         <f t="shared" ca="1" si="12"/>
@@ -4742,25 +4742,25 @@
         <f t="shared" ca="1" si="10"/>
         <v/>
       </c>
-      <c r="AC17" s="12" t="str">
+      <c r="AC17" s="12">
         <f t="shared" ca="1" si="11"/>
-        <v/>
-      </c>
-      <c r="AD17" s="12" t="str">
+        <v>2</v>
+      </c>
+      <c r="AD17" s="12">
         <f t="shared" ca="1" si="11"/>
-        <v/>
-      </c>
-      <c r="AE17" s="12" t="str">
+        <v>2</v>
+      </c>
+      <c r="AE17" s="12">
         <f t="shared" ca="1" si="11"/>
-        <v/>
-      </c>
-      <c r="AF17" s="12" t="str">
+        <v>2</v>
+      </c>
+      <c r="AF17" s="12">
         <f t="shared" ca="1" si="11"/>
-        <v/>
-      </c>
-      <c r="AG17" s="12" t="str">
+        <v>2</v>
+      </c>
+      <c r="AG17" s="12">
         <f t="shared" ca="1" si="11"/>
-        <v/>
+        <v>2</v>
       </c>
       <c r="AH17" s="12">
         <f t="shared" ca="1" si="11"/>
@@ -4798,25 +4798,25 @@
         <f t="shared" ca="1" si="12"/>
         <v>2</v>
       </c>
-      <c r="AQ17" s="12">
+      <c r="AQ17" s="12" t="str">
         <f t="shared" ca="1" si="12"/>
-        <v>2</v>
-      </c>
-      <c r="AR17" s="12">
+        <v/>
+      </c>
+      <c r="AR17" s="12" t="str">
         <f t="shared" ca="1" si="12"/>
-        <v>2</v>
-      </c>
-      <c r="AS17" s="12">
+        <v/>
+      </c>
+      <c r="AS17" s="12" t="str">
         <f t="shared" ca="1" si="12"/>
-        <v>2</v>
-      </c>
-      <c r="AT17" s="12">
+        <v/>
+      </c>
+      <c r="AT17" s="12" t="str">
         <f t="shared" ca="1" si="12"/>
-        <v>2</v>
-      </c>
-      <c r="AU17" s="12">
+        <v/>
+      </c>
+      <c r="AU17" s="12" t="str">
         <f t="shared" ca="1" si="12"/>
-        <v>2</v>
+        <v/>
       </c>
       <c r="AV17" s="12" t="str">
         <f t="shared" ca="1" si="12"/>
@@ -5068,25 +5068,25 @@
         <f t="shared" ca="1" si="13"/>
         <v/>
       </c>
-      <c r="AX18" s="12" t="str">
+      <c r="AX18" s="12">
         <f t="shared" ca="1" si="13"/>
-        <v/>
-      </c>
-      <c r="AY18" s="12" t="str">
+        <v>2</v>
+      </c>
+      <c r="AY18" s="12">
         <f t="shared" ca="1" si="13"/>
-        <v/>
-      </c>
-      <c r="AZ18" s="12" t="str">
+        <v>2</v>
+      </c>
+      <c r="AZ18" s="12">
         <f t="shared" ca="1" si="13"/>
-        <v/>
-      </c>
-      <c r="BA18" s="12" t="str">
+        <v>2</v>
+      </c>
+      <c r="BA18" s="12">
         <f t="shared" ca="1" si="13"/>
-        <v/>
-      </c>
-      <c r="BB18" s="12" t="str">
+        <v>2</v>
+      </c>
+      <c r="BB18" s="12">
         <f t="shared" ca="1" si="13"/>
-        <v/>
+        <v>2</v>
       </c>
       <c r="BC18" s="12">
         <f t="shared" ca="1" si="13"/>
@@ -6208,21 +6208,21 @@
         <v>11</v>
       </c>
       <c r="H24" s="15"/>
-      <c r="I24" s="12">
+      <c r="I24" s="12" t="str">
         <f t="shared" ref="I24:R30" ca="1" si="15">IF(AND($C24="Doel",I$7&gt;=$F24,I$7&lt;=$F24+$G24-1),2,IF(AND($C24="Mijlpaal",I$7&gt;=$F24,I$7&lt;=$F24+$G24-1),1,""))</f>
-        <v>1</v>
-      </c>
-      <c r="J24" s="12">
+        <v/>
+      </c>
+      <c r="J24" s="12" t="str">
         <f t="shared" ca="1" si="15"/>
-        <v>1</v>
-      </c>
-      <c r="K24" s="12">
+        <v/>
+      </c>
+      <c r="K24" s="12" t="str">
         <f t="shared" ca="1" si="15"/>
-        <v>1</v>
-      </c>
-      <c r="L24" s="12">
+        <v/>
+      </c>
+      <c r="L24" s="12" t="str">
         <f t="shared" ca="1" si="15"/>
-        <v>1</v>
+        <v/>
       </c>
       <c r="M24" s="12" t="str">
         <f t="shared" ca="1" si="15"/>
@@ -6452,21 +6452,21 @@
         <v>14</v>
       </c>
       <c r="H25" s="15"/>
-      <c r="I25" s="12" t="str">
+      <c r="I25" s="12">
         <f t="shared" ca="1" si="15"/>
-        <v/>
-      </c>
-      <c r="J25" s="12" t="str">
+        <v>2</v>
+      </c>
+      <c r="J25" s="12">
         <f t="shared" ca="1" si="15"/>
-        <v/>
-      </c>
-      <c r="K25" s="12" t="str">
+        <v>2</v>
+      </c>
+      <c r="K25" s="12">
         <f t="shared" ca="1" si="15"/>
-        <v/>
-      </c>
-      <c r="L25" s="12" t="str">
+        <v>2</v>
+      </c>
+      <c r="L25" s="12">
         <f t="shared" ca="1" si="15"/>
-        <v/>
+        <v>2</v>
       </c>
       <c r="M25" s="12">
         <f t="shared" ca="1" si="15"/>
@@ -6504,25 +6504,25 @@
         <f t="shared" ca="1" si="16"/>
         <v>2</v>
       </c>
-      <c r="V25" s="12">
+      <c r="V25" s="12" t="str">
         <f t="shared" ca="1" si="16"/>
-        <v>2</v>
-      </c>
-      <c r="W25" s="12">
+        <v/>
+      </c>
+      <c r="W25" s="12" t="str">
         <f t="shared" ca="1" si="16"/>
-        <v>2</v>
-      </c>
-      <c r="X25" s="12">
+        <v/>
+      </c>
+      <c r="X25" s="12" t="str">
         <f t="shared" ca="1" si="16"/>
-        <v>2</v>
-      </c>
-      <c r="Y25" s="12">
+        <v/>
+      </c>
+      <c r="Y25" s="12" t="str">
         <f t="shared" ca="1" si="16"/>
-        <v>2</v>
-      </c>
-      <c r="Z25" s="12">
+        <v/>
+      </c>
+      <c r="Z25" s="12" t="str">
         <f t="shared" ca="1" si="16"/>
-        <v>2</v>
+        <v/>
       </c>
       <c r="AA25" s="12" t="str">
         <f t="shared" ca="1" si="16"/>
@@ -6704,25 +6704,25 @@
         <f t="shared" ca="1" si="15"/>
         <v>1</v>
       </c>
-      <c r="K26" s="12">
+      <c r="K26" s="12" t="str">
         <f t="shared" ca="1" si="15"/>
-        <v>1</v>
-      </c>
-      <c r="L26" s="12">
+        <v/>
+      </c>
+      <c r="L26" s="12" t="str">
         <f t="shared" ca="1" si="15"/>
-        <v>1</v>
-      </c>
-      <c r="M26" s="12">
+        <v/>
+      </c>
+      <c r="M26" s="12" t="str">
         <f t="shared" ca="1" si="15"/>
-        <v>1</v>
-      </c>
-      <c r="N26" s="12">
+        <v/>
+      </c>
+      <c r="N26" s="12" t="str">
         <f t="shared" ca="1" si="15"/>
-        <v>1</v>
-      </c>
-      <c r="O26" s="12">
+        <v/>
+      </c>
+      <c r="O26" s="12" t="str">
         <f t="shared" ca="1" si="15"/>
-        <v>1</v>
+        <v/>
       </c>
       <c r="P26" s="12" t="str">
         <f t="shared" ca="1" si="15"/>
@@ -6942,21 +6942,21 @@
         <v>11</v>
       </c>
       <c r="H27" s="15"/>
-      <c r="I27" s="12">
+      <c r="I27" s="12" t="str">
         <f t="shared" ca="1" si="15"/>
-        <v>2</v>
-      </c>
-      <c r="J27" s="12">
+        <v/>
+      </c>
+      <c r="J27" s="12" t="str">
         <f t="shared" ca="1" si="15"/>
-        <v>2</v>
-      </c>
-      <c r="K27" s="12">
+        <v/>
+      </c>
+      <c r="K27" s="12" t="str">
         <f t="shared" ca="1" si="15"/>
-        <v>2</v>
-      </c>
-      <c r="L27" s="12">
+        <v/>
+      </c>
+      <c r="L27" s="12" t="str">
         <f t="shared" ca="1" si="15"/>
-        <v>2</v>
+        <v/>
       </c>
       <c r="M27" s="12" t="str">
         <f t="shared" ca="1" si="15"/>
@@ -7432,21 +7432,21 @@
         <v>4</v>
       </c>
       <c r="H29" s="15"/>
-      <c r="I29" s="12">
+      <c r="I29" s="12" t="str">
         <f t="shared" ca="1" si="15"/>
-        <v>1</v>
-      </c>
-      <c r="J29" s="12">
+        <v/>
+      </c>
+      <c r="J29" s="12" t="str">
         <f t="shared" ca="1" si="15"/>
-        <v>1</v>
-      </c>
-      <c r="K29" s="12">
+        <v/>
+      </c>
+      <c r="K29" s="12" t="str">
         <f t="shared" ca="1" si="15"/>
-        <v>1</v>
-      </c>
-      <c r="L29" s="12">
+        <v/>
+      </c>
+      <c r="L29" s="12" t="str">
         <f t="shared" ca="1" si="15"/>
-        <v>1</v>
+        <v/>
       </c>
       <c r="M29" s="12" t="str">
         <f t="shared" ca="1" si="15"/>
@@ -8546,25 +8546,25 @@
         <f t="shared" ca="1" si="23"/>
         <v/>
       </c>
-      <c r="K37" s="12" t="str">
+      <c r="K37" s="12">
         <f t="shared" ca="1" si="23"/>
-        <v/>
-      </c>
-      <c r="L37" s="12" t="str">
+        <v>1</v>
+      </c>
+      <c r="L37" s="12">
         <f t="shared" ca="1" si="23"/>
-        <v/>
-      </c>
-      <c r="M37" s="12" t="str">
+        <v>1</v>
+      </c>
+      <c r="M37" s="12">
         <f t="shared" ca="1" si="23"/>
-        <v/>
-      </c>
-      <c r="N37" s="12" t="str">
+        <v>1</v>
+      </c>
+      <c r="N37" s="12">
         <f t="shared" ca="1" si="23"/>
-        <v/>
-      </c>
-      <c r="O37" s="12" t="str">
+        <v>1</v>
+      </c>
+      <c r="O37" s="12">
         <f t="shared" ca="1" si="23"/>
-        <v/>
+        <v>1</v>
       </c>
       <c r="P37" s="12">
         <f t="shared" ca="1" si="23"/>
@@ -8618,25 +8618,25 @@
         <f t="shared" ca="1" si="24"/>
         <v>1</v>
       </c>
-      <c r="AC37" s="12">
+      <c r="AC37" s="12" t="str">
         <f t="shared" ref="AC37:AL39" ca="1" si="25">IF(AND($C37="Doel",AC$7&gt;=$F37,AC$7&lt;=$F37+$G37-1),2,IF(AND($C37="Mijlpaal",AC$7&gt;=$F37,AC$7&lt;=$F37+$G37-1),1,""))</f>
-        <v>1</v>
-      </c>
-      <c r="AD37" s="12">
+        <v/>
+      </c>
+      <c r="AD37" s="12" t="str">
         <f t="shared" ca="1" si="25"/>
-        <v>1</v>
-      </c>
-      <c r="AE37" s="12">
+        <v/>
+      </c>
+      <c r="AE37" s="12" t="str">
         <f t="shared" ca="1" si="25"/>
-        <v>1</v>
-      </c>
-      <c r="AF37" s="12">
+        <v/>
+      </c>
+      <c r="AF37" s="12" t="str">
         <f t="shared" ca="1" si="25"/>
-        <v>1</v>
-      </c>
-      <c r="AG37" s="12">
+        <v/>
+      </c>
+      <c r="AG37" s="12" t="str">
         <f t="shared" ca="1" si="25"/>
-        <v>1</v>
+        <v/>
       </c>
       <c r="AH37" s="12" t="str">
         <f t="shared" ca="1" si="25"/>
@@ -9110,49 +9110,49 @@
         <f t="shared" ca="1" si="25"/>
         <v/>
       </c>
-      <c r="AF39" s="12" t="str">
+      <c r="AF39" s="12">
         <f t="shared" ca="1" si="25"/>
-        <v/>
-      </c>
-      <c r="AG39" s="12" t="str">
+        <v>1</v>
+      </c>
+      <c r="AG39" s="12">
         <f t="shared" ca="1" si="25"/>
-        <v/>
-      </c>
-      <c r="AH39" s="12" t="str">
+        <v>1</v>
+      </c>
+      <c r="AH39" s="12">
         <f t="shared" ca="1" si="25"/>
-        <v/>
-      </c>
-      <c r="AI39" s="12" t="str">
+        <v>1</v>
+      </c>
+      <c r="AI39" s="12">
         <f t="shared" ca="1" si="25"/>
-        <v/>
-      </c>
-      <c r="AJ39" s="12" t="str">
+        <v>1</v>
+      </c>
+      <c r="AJ39" s="12">
         <f t="shared" ca="1" si="25"/>
-        <v/>
+        <v>1</v>
       </c>
       <c r="AK39" s="12">
         <f t="shared" ca="1" si="25"/>
         <v>1</v>
       </c>
-      <c r="AL39" s="12">
+      <c r="AL39" s="12" t="str">
         <f t="shared" ca="1" si="25"/>
-        <v>1</v>
-      </c>
-      <c r="AM39" s="12">
+        <v/>
+      </c>
+      <c r="AM39" s="12" t="str">
         <f t="shared" ca="1" si="26"/>
-        <v>1</v>
-      </c>
-      <c r="AN39" s="12">
+        <v/>
+      </c>
+      <c r="AN39" s="12" t="str">
         <f t="shared" ca="1" si="26"/>
-        <v>1</v>
-      </c>
-      <c r="AO39" s="12">
+        <v/>
+      </c>
+      <c r="AO39" s="12" t="str">
         <f t="shared" ca="1" si="26"/>
-        <v>1</v>
-      </c>
-      <c r="AP39" s="12">
+        <v/>
+      </c>
+      <c r="AP39" s="12" t="str">
         <f t="shared" ca="1" si="26"/>
-        <v>1</v>
+        <v/>
       </c>
       <c r="AQ39" s="12" t="str">
         <f t="shared" ca="1" si="26"/>
@@ -10239,6 +10239,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010079F111ED35F8CC479449609E8A0923A6" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="22a266b9fa9a230c5a512669d8b298c3">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xmlns:ns3="16c05727-aa75-4e4a-9b5f-8a80a1165891" xmlns:ns4="230e9df3-be65-4c73-a93b-d1236ebd677e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="eddc33fff6b14141ee5c74a0d29ea6a1" ns1:_="" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -10514,15 +10523,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AA4BA2A8-DB97-40F9-8DB6-154C09C7467C}">
   <ds:schemaRefs>
@@ -10536,6 +10536,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{39060724-9CA2-4290-8A0C-B53624A594E7}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{75C87518-DD8E-42CD-8DAC-291A323E849B}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -10554,12 +10562,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{39060724-9CA2-4290-8A0C-B53624A594E7}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
seminaries documentatie: excel planning, temp bom lijst in foot prints en stakeholder analyse
</commit_message>
<xml_diff>
--- a/Super Epische Audio Generator/Seminaries/planning_audio_generator.xlsx
+++ b/Super Epische Audio Generator/Seminaries/planning_audio_generator.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{597340E0-799B-4801-B28C-E1C9822D9F32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" tabRatio="415"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="415" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="planning " sheetId="17" r:id="rId1"/>
@@ -15,7 +16,7 @@
     <definedName name="Scrolverhoging" localSheetId="0">'planning '!$C$7</definedName>
     <definedName name="Vandaag" localSheetId="0">TODAY()</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -27,6 +28,8 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -34,14 +37,14 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
   <futureMetadata name="XLDAPR" count="1">
     <bk>
       <extLst>
-        <ext xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray" uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
           <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
         </ext>
       </extLst>
@@ -56,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="68">
   <si>
     <t>Begindatum project:</t>
   </si>
@@ -184,16 +187,10 @@
     <t>Iedereen</t>
   </si>
   <si>
-    <t xml:space="preserve">PCB ontwerpen </t>
-  </si>
-  <si>
     <t>Fase 2 (07/03)</t>
   </si>
   <si>
     <t>FASE 1 (29/02)</t>
-  </si>
-  <si>
-    <t>buizingen tekenen en printen</t>
   </si>
   <si>
     <t xml:space="preserve">Finale I/O beslissingen maken </t>
@@ -217,12 +214,6 @@
     <t xml:space="preserve">Codec randapparaten </t>
   </si>
   <si>
-    <t>Fase 3 (28/03)</t>
-  </si>
-  <si>
-    <t>buffer periode voor eventueel werk in te halen</t>
-  </si>
-  <si>
     <t>Seppe en Joran</t>
   </si>
   <si>
@@ -235,19 +226,49 @@
     <t xml:space="preserve">* meerdere inputs implementeren </t>
   </si>
   <si>
-    <t>Fase 4 (1/04 Paasvakantie)</t>
-  </si>
-  <si>
     <t xml:space="preserve"> pcb maken </t>
   </si>
   <si>
     <t xml:space="preserve">behuizing afwerken </t>
   </si>
+  <si>
+    <t>Seppe en Floran</t>
+  </si>
+  <si>
+    <t>%</t>
+  </si>
+  <si>
+    <t>Buffer periode voor eventueel werk in te halen</t>
+  </si>
+  <si>
+    <t>PCB Designen</t>
+  </si>
+  <si>
+    <t>wachten op PCB levering</t>
+  </si>
+  <si>
+    <t>Behuizing tekenen en printen</t>
+  </si>
+  <si>
+    <t>PCB</t>
+  </si>
+  <si>
+    <t>Pcb bestukken</t>
+  </si>
+  <si>
+    <t>behuizing monteren</t>
+  </si>
+  <si>
+    <t>Fase 3 (28/03 &amp; 1/04 Paasvakantie)</t>
+  </si>
+  <si>
+    <t>Fase 4 (10/04)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <numFmts count="5">
     <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="165" formatCode="_-&quot;kr&quot;\ * #,##0.00_-;\-&quot;kr&quot;\ * #,##0.00_-;_-&quot;kr&quot;\ * &quot;-&quot;??_-;_-@_-"/>
@@ -255,7 +276,7 @@
     <numFmt numFmtId="167" formatCode="#,##0_ ;\-#,##0\ "/>
     <numFmt numFmtId="168" formatCode="d"/>
   </numFmts>
-  <fonts count="35" x14ac:knownFonts="1">
+  <fonts count="37" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -506,6 +527,17 @@
       <sz val="18"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -1212,11 +1244,8 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1" indent="3"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="9" applyFont="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1224,15 +1253,20 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="167" fontId="9" fillId="0" borderId="0" xfId="10" applyFont="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="9" fontId="36" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="35" fillId="0" borderId="0" xfId="9" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="35" fillId="0" borderId="0" xfId="10" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1284,34 +1318,34 @@
     <cellStyle name="Accent4" xfId="38" builtinId="41" customBuiltin="1"/>
     <cellStyle name="Accent5" xfId="42" builtinId="45" customBuiltin="1"/>
     <cellStyle name="Accent6" xfId="46" builtinId="49" customBuiltin="1"/>
-    <cellStyle name="Bad" xfId="16" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="Calculation" xfId="20" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="Check Cell" xfId="22" builtinId="23" customBuiltin="1"/>
-    <cellStyle name="Comma" xfId="4" builtinId="3" customBuiltin="1"/>
-    <cellStyle name="Comma [0]" xfId="10" builtinId="6" customBuiltin="1"/>
-    <cellStyle name="Currency" xfId="12" builtinId="4" customBuiltin="1"/>
-    <cellStyle name="Currency [0]" xfId="13" builtinId="7" customBuiltin="1"/>
-    <cellStyle name="Datum" xfId="9"/>
-    <cellStyle name="Explanatory Text" xfId="25" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="Good" xfId="15" builtinId="26" customBuiltin="1"/>
-    <cellStyle name="Heading 1" xfId="6" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Heading 2" xfId="7" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Heading 3" xfId="8" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="Heading 4" xfId="14" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Berekening" xfId="20" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Controlecel" xfId="22" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Datum" xfId="9" xr:uid="{00000000-0005-0000-0000-00001F000000}"/>
+    <cellStyle name="Gekoppelde cel" xfId="21" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="Goed" xfId="15" builtinId="26" customBuiltin="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" customBuiltin="1"/>
-    <cellStyle name="Input" xfId="18" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="Linked Cell" xfId="21" builtinId="24" customBuiltin="1"/>
-    <cellStyle name="Neutral" xfId="17" builtinId="28" customBuiltin="1"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
-    <cellStyle name="Note" xfId="24" builtinId="10" customBuiltin="1"/>
-    <cellStyle name="Output" xfId="19" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="Percent" xfId="2" builtinId="5" customBuiltin="1"/>
-    <cellStyle name="Title" xfId="5" builtinId="15" customBuiltin="1"/>
-    <cellStyle name="Total" xfId="26" builtinId="25" customBuiltin="1"/>
-    <cellStyle name="Warning Text" xfId="23" builtinId="11" customBuiltin="1"/>
-    <cellStyle name="zHiddenText" xfId="3"/>
+    <cellStyle name="Invoer" xfId="18" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Komma" xfId="4" builtinId="3" customBuiltin="1"/>
+    <cellStyle name="Komma [0]" xfId="10" builtinId="6" customBuiltin="1"/>
+    <cellStyle name="Kop 1" xfId="6" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Kop 2" xfId="7" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Kop 3" xfId="8" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Kop 4" xfId="14" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Neutraal" xfId="17" builtinId="28" customBuiltin="1"/>
+    <cellStyle name="Notitie" xfId="24" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Ongeldig" xfId="16" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Procent" xfId="2" builtinId="5" customBuiltin="1"/>
+    <cellStyle name="Standaard" xfId="0" builtinId="0" customBuiltin="1"/>
+    <cellStyle name="Titel" xfId="5" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Totaal" xfId="26" builtinId="25" customBuiltin="1"/>
+    <cellStyle name="Uitvoer" xfId="19" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Valuta" xfId="12" builtinId="4" customBuiltin="1"/>
+    <cellStyle name="Valuta [0]" xfId="13" builtinId="7" customBuiltin="1"/>
+    <cellStyle name="Verklarende tekst" xfId="25" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Waarschuwingstekst" xfId="23" builtinId="11" customBuiltin="1"/>
+    <cellStyle name="zHiddenText" xfId="3" xr:uid="{00000000-0005-0000-0000-000031000000}"/>
   </cellStyles>
-  <dxfs count="40">
+  <dxfs count="50">
     <dxf>
       <font>
         <strike val="0"/>
@@ -1418,6 +1452,144 @@
           <bgColor theme="1" tint="0.249977111117893"/>
         </patternFill>
       </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="2" tint="-9.9948118533890809E-2"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="2" tint="-9.9948118533890809E-2"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
     </dxf>
     <dxf>
       <fill>
@@ -1869,22 +2041,22 @@
     </dxf>
   </dxfs>
   <tableStyles count="2" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="Gantt-tabelstijl" pivot="0" count="4">
-      <tableStyleElement type="wholeTable" dxfId="39"/>
-      <tableStyleElement type="headerRow" dxfId="38"/>
-      <tableStyleElement type="firstRowStripe" dxfId="37"/>
-      <tableStyleElement type="secondRowStripe" dxfId="36"/>
+    <tableStyle name="Gantt-tabelstijl" pivot="0" count="4" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
+      <tableStyleElement type="wholeTable" dxfId="49"/>
+      <tableStyleElement type="headerRow" dxfId="48"/>
+      <tableStyleElement type="firstRowStripe" dxfId="47"/>
+      <tableStyleElement type="secondRowStripe" dxfId="46"/>
     </tableStyle>
-    <tableStyle name="Takenlijst" pivot="0" count="9">
-      <tableStyleElement type="wholeTable" dxfId="35"/>
-      <tableStyleElement type="headerRow" dxfId="34"/>
-      <tableStyleElement type="totalRow" dxfId="33"/>
-      <tableStyleElement type="firstColumn" dxfId="32"/>
-      <tableStyleElement type="lastColumn" dxfId="31"/>
-      <tableStyleElement type="firstRowStripe" dxfId="30"/>
-      <tableStyleElement type="secondRowStripe" dxfId="29"/>
-      <tableStyleElement type="firstColumnStripe" dxfId="28"/>
-      <tableStyleElement type="secondColumnStripe" dxfId="27"/>
+    <tableStyle name="Takenlijst" pivot="0" count="9" xr9:uid="{00000000-0011-0000-FFFF-FFFF01000000}">
+      <tableStyleElement type="wholeTable" dxfId="45"/>
+      <tableStyleElement type="headerRow" dxfId="44"/>
+      <tableStyleElement type="totalRow" dxfId="43"/>
+      <tableStyleElement type="firstColumn" dxfId="42"/>
+      <tableStyleElement type="lastColumn" dxfId="41"/>
+      <tableStyleElement type="firstRowStripe" dxfId="40"/>
+      <tableStyleElement type="secondRowStripe" dxfId="39"/>
+      <tableStyleElement type="firstColumnStripe" dxfId="38"/>
+      <tableStyleElement type="secondColumnStripe" dxfId="37"/>
     </tableStyle>
   </tableStyles>
   <colors>
@@ -1955,8 +2127,8 @@
       <rgbColor rgb="00333333"/>
     </indexedColors>
     <mruColors>
+      <color rgb="FF215881"/>
       <color rgb="FF000000"/>
-      <color rgb="FF215881"/>
       <color rgb="FF42648A"/>
       <color rgb="FF969696"/>
       <color rgb="FFC0C0C0"/>
@@ -1978,7 +2150,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp1.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Scroll" dx="39" fmlaLink="$C$7" horiz="1" max="365" page="2" val="0"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Scroll" dx="39" fmlaLink="$C$7" horiz="1" max="365" page="2" val="4"/>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1988,15 +2160,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>8</xdr:col>
-          <xdr:colOff>28575</xdr:colOff>
+          <xdr:colOff>30480</xdr:colOff>
           <xdr:row>7</xdr:row>
-          <xdr:rowOff>57150</xdr:rowOff>
+          <xdr:rowOff>60960</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>63</xdr:col>
           <xdr:colOff>228600</xdr:colOff>
           <xdr:row>7</xdr:row>
-          <xdr:rowOff>238125</xdr:rowOff>
+          <xdr:rowOff>236220</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -2037,8 +2209,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Milestones4352" displayName="Milestones4352" ref="B9:G48" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
-  <autoFilter ref="B9:G48">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Milestones4352" displayName="Milestones4352" ref="B9:G51" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
+  <autoFilter ref="B9:G51" xr:uid="{00000000-0009-0000-0100-000001000000}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -2047,12 +2219,12 @@
     <filterColumn colId="5" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="6">
-    <tableColumn id="1" name="Mijlpaalbeschrijving" dataDxfId="5"/>
-    <tableColumn id="2" name="Categorie" dataDxfId="4"/>
-    <tableColumn id="3" name="Toegewezen aan" dataDxfId="3"/>
-    <tableColumn id="4" name="Voortgang" dataDxfId="2"/>
-    <tableColumn id="5" name="Start" dataDxfId="1" dataCellStyle="Datum"/>
-    <tableColumn id="6" name="Dagen" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Mijlpaalbeschrijving" dataDxfId="5"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Categorie" dataDxfId="4"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Toegewezen aan" dataDxfId="3"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Voortgang" dataDxfId="2"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Start" dataDxfId="1" dataCellStyle="Datum"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Dagen" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="Takenlijst" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
   <extLst>
@@ -2325,29 +2497,29 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BP49"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:BP52"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" showRuler="0" topLeftCell="A29" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
-      <selection activeCell="D33" sqref="D33"/>
+    <sheetView showGridLines="0" tabSelected="1" showRuler="0" topLeftCell="A35" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="70" workbookViewId="0">
+      <selection activeCell="F47" sqref="F47"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="4.7109375" style="5" customWidth="1"/>
-    <col min="2" max="2" width="42.5703125" customWidth="1"/>
-    <col min="3" max="3" width="17.140625" customWidth="1"/>
-    <col min="4" max="4" width="20.5703125" customWidth="1"/>
-    <col min="5" max="5" width="15.7109375" customWidth="1"/>
-    <col min="6" max="6" width="10.42578125" style="2" customWidth="1"/>
-    <col min="7" max="7" width="10.42578125" customWidth="1"/>
-    <col min="8" max="8" width="2.7109375" customWidth="1"/>
-    <col min="9" max="64" width="3.5703125" customWidth="1"/>
-    <col min="65" max="65" width="2.7109375" customWidth="1"/>
+    <col min="1" max="1" width="4.6640625" style="5" customWidth="1"/>
+    <col min="2" max="2" width="55.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.109375" customWidth="1"/>
+    <col min="4" max="4" width="20.5546875" customWidth="1"/>
+    <col min="5" max="5" width="15.6640625" customWidth="1"/>
+    <col min="6" max="6" width="10.44140625" style="2" customWidth="1"/>
+    <col min="7" max="7" width="10.44140625" customWidth="1"/>
+    <col min="8" max="8" width="2.6640625" customWidth="1"/>
+    <col min="9" max="64" width="3.5546875" customWidth="1"/>
+    <col min="65" max="65" width="2.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:68" ht="25.15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="1:68" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:68" ht="25.2" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="1:68" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="6"/>
       <c r="B2" s="72" t="s">
         <v>23</v>
@@ -2416,7 +2588,7 @@
       <c r="BL2" s="20"/>
       <c r="BM2" s="20"/>
     </row>
-    <row r="3" spans="1:68" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:68" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="6"/>
       <c r="B3" s="21"/>
       <c r="C3" s="22"/>
@@ -2430,7 +2602,7 @@
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
     </row>
-    <row r="4" spans="1:68" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:68" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="6"/>
       <c r="B4" s="25"/>
       <c r="C4" s="26"/>
@@ -2476,7 +2648,7 @@
       <c r="AI4" s="71"/>
       <c r="AJ4" s="71"/>
     </row>
-    <row r="5" spans="1:68" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:68" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="6"/>
       <c r="B5" s="31"/>
       <c r="C5" s="27"/>
@@ -2486,14 +2658,14 @@
       <c r="G5" s="28"/>
       <c r="H5" s="28"/>
     </row>
-    <row r="6" spans="1:68" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:68" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A6" s="6"/>
       <c r="B6" s="32" t="s">
         <v>0</v>
       </c>
       <c r="C6" s="33" cm="1">
         <f t="array" aca="1" ref="C6" ca="1">IFERROR(IF(MIN(Milestones4352[Start])=0,TODAY(),B11(Milestones4352[Start])),TODAY())</f>
-        <v>45356</v>
+        <v>45358</v>
       </c>
       <c r="D6" s="34"/>
       <c r="E6" s="28"/>
@@ -2502,7 +2674,7 @@
       <c r="H6" s="28"/>
       <c r="I6" s="44" t="str">
         <f ca="1">TEXT(I7,"mmmm")</f>
-        <v>March</v>
+        <v>maart</v>
       </c>
       <c r="J6" s="44"/>
       <c r="K6" s="44"/>
@@ -2532,7 +2704,7 @@
       <c r="AC6" s="44"/>
       <c r="AD6" s="44" t="str">
         <f ca="1">IF(OR(TEXT(AD7,"mmmm")=W6,TEXT(AD7,"mmmm")=P6,TEXT(AD7,"mmmm")=I6),"",TEXT(AD7,"mmmm"))</f>
-        <v/>
+        <v>april</v>
       </c>
       <c r="AE6" s="44"/>
       <c r="AF6" s="44"/>
@@ -2542,7 +2714,7 @@
       <c r="AJ6" s="44"/>
       <c r="AK6" s="44" t="str">
         <f ca="1">IF(OR(TEXT(AK7,"mmmm")=AD6,TEXT(AK7,"mmmm")=W6,TEXT(AK7,"mmmm")=P6,TEXT(AK7,"mmmm")=I6),"",TEXT(AK7,"mmmm"))</f>
-        <v>April</v>
+        <v/>
       </c>
       <c r="AL6" s="44"/>
       <c r="AM6" s="44"/>
@@ -2581,13 +2753,13 @@
       <c r="BK6" s="43"/>
       <c r="BL6" s="43"/>
     </row>
-    <row r="7" spans="1:68" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:68" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="6"/>
       <c r="B7" s="32" t="s">
         <v>1</v>
       </c>
       <c r="C7" s="35">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D7" s="27"/>
       <c r="E7" s="28"/>
@@ -2596,230 +2768,230 @@
       <c r="H7" s="36"/>
       <c r="I7" s="51">
         <f ca="1">IFERROR(Project_Start+Scrolverhoging,TODAY())</f>
-        <v>45356</v>
+        <v>45362</v>
       </c>
       <c r="J7" s="52">
         <f ca="1">I7+1</f>
-        <v>45357</v>
+        <v>45363</v>
       </c>
       <c r="K7" s="52">
         <f t="shared" ref="K7:AX7" ca="1" si="0">J7+1</f>
-        <v>45358</v>
+        <v>45364</v>
       </c>
       <c r="L7" s="52">
         <f t="shared" ca="1" si="0"/>
-        <v>45359</v>
+        <v>45365</v>
       </c>
       <c r="M7" s="52">
         <f t="shared" ca="1" si="0"/>
-        <v>45360</v>
+        <v>45366</v>
       </c>
       <c r="N7" s="52">
         <f t="shared" ca="1" si="0"/>
-        <v>45361</v>
+        <v>45367</v>
       </c>
       <c r="O7" s="53">
         <f t="shared" ca="1" si="0"/>
-        <v>45362</v>
+        <v>45368</v>
       </c>
       <c r="P7" s="52">
         <f ca="1">O7+1</f>
-        <v>45363</v>
+        <v>45369</v>
       </c>
       <c r="Q7" s="52">
         <f ca="1">P7+1</f>
-        <v>45364</v>
+        <v>45370</v>
       </c>
       <c r="R7" s="52">
         <f t="shared" ca="1" si="0"/>
-        <v>45365</v>
+        <v>45371</v>
       </c>
       <c r="S7" s="52">
         <f t="shared" ca="1" si="0"/>
-        <v>45366</v>
+        <v>45372</v>
       </c>
       <c r="T7" s="52">
         <f t="shared" ca="1" si="0"/>
-        <v>45367</v>
+        <v>45373</v>
       </c>
       <c r="U7" s="52">
         <f t="shared" ca="1" si="0"/>
-        <v>45368</v>
+        <v>45374</v>
       </c>
       <c r="V7" s="53">
         <f t="shared" ca="1" si="0"/>
-        <v>45369</v>
+        <v>45375</v>
       </c>
       <c r="W7" s="52">
         <f ca="1">V7+1</f>
-        <v>45370</v>
+        <v>45376</v>
       </c>
       <c r="X7" s="52">
         <f ca="1">W7+1</f>
-        <v>45371</v>
+        <v>45377</v>
       </c>
       <c r="Y7" s="52">
         <f t="shared" ca="1" si="0"/>
-        <v>45372</v>
+        <v>45378</v>
       </c>
       <c r="Z7" s="52">
         <f t="shared" ca="1" si="0"/>
-        <v>45373</v>
+        <v>45379</v>
       </c>
       <c r="AA7" s="52">
         <f t="shared" ca="1" si="0"/>
-        <v>45374</v>
+        <v>45380</v>
       </c>
       <c r="AB7" s="52">
         <f t="shared" ca="1" si="0"/>
-        <v>45375</v>
+        <v>45381</v>
       </c>
       <c r="AC7" s="53">
         <f t="shared" ca="1" si="0"/>
-        <v>45376</v>
+        <v>45382</v>
       </c>
       <c r="AD7" s="52">
         <f ca="1">AC7+1</f>
-        <v>45377</v>
+        <v>45383</v>
       </c>
       <c r="AE7" s="52">
         <f ca="1">AD7+1</f>
-        <v>45378</v>
+        <v>45384</v>
       </c>
       <c r="AF7" s="52">
         <f t="shared" ca="1" si="0"/>
-        <v>45379</v>
+        <v>45385</v>
       </c>
       <c r="AG7" s="52">
         <f t="shared" ca="1" si="0"/>
-        <v>45380</v>
+        <v>45386</v>
       </c>
       <c r="AH7" s="52">
         <f t="shared" ca="1" si="0"/>
-        <v>45381</v>
+        <v>45387</v>
       </c>
       <c r="AI7" s="52">
         <f t="shared" ca="1" si="0"/>
-        <v>45382</v>
+        <v>45388</v>
       </c>
       <c r="AJ7" s="53">
         <f t="shared" ca="1" si="0"/>
-        <v>45383</v>
+        <v>45389</v>
       </c>
       <c r="AK7" s="52">
         <f ca="1">AJ7+1</f>
-        <v>45384</v>
+        <v>45390</v>
       </c>
       <c r="AL7" s="52">
         <f ca="1">AK7+1</f>
-        <v>45385</v>
+        <v>45391</v>
       </c>
       <c r="AM7" s="52">
         <f t="shared" ca="1" si="0"/>
-        <v>45386</v>
+        <v>45392</v>
       </c>
       <c r="AN7" s="52">
         <f t="shared" ca="1" si="0"/>
-        <v>45387</v>
+        <v>45393</v>
       </c>
       <c r="AO7" s="52">
         <f t="shared" ca="1" si="0"/>
-        <v>45388</v>
+        <v>45394</v>
       </c>
       <c r="AP7" s="52">
         <f t="shared" ca="1" si="0"/>
-        <v>45389</v>
+        <v>45395</v>
       </c>
       <c r="AQ7" s="53">
         <f t="shared" ca="1" si="0"/>
-        <v>45390</v>
+        <v>45396</v>
       </c>
       <c r="AR7" s="52">
         <f ca="1">AQ7+1</f>
-        <v>45391</v>
+        <v>45397</v>
       </c>
       <c r="AS7" s="52">
         <f ca="1">AR7+1</f>
-        <v>45392</v>
+        <v>45398</v>
       </c>
       <c r="AT7" s="52">
         <f t="shared" ca="1" si="0"/>
-        <v>45393</v>
+        <v>45399</v>
       </c>
       <c r="AU7" s="52">
         <f t="shared" ca="1" si="0"/>
-        <v>45394</v>
+        <v>45400</v>
       </c>
       <c r="AV7" s="52">
         <f t="shared" ca="1" si="0"/>
-        <v>45395</v>
+        <v>45401</v>
       </c>
       <c r="AW7" s="52">
         <f t="shared" ca="1" si="0"/>
-        <v>45396</v>
+        <v>45402</v>
       </c>
       <c r="AX7" s="53">
         <f t="shared" ca="1" si="0"/>
-        <v>45397</v>
+        <v>45403</v>
       </c>
       <c r="AY7" s="52">
         <f ca="1">AX7+1</f>
-        <v>45398</v>
+        <v>45404</v>
       </c>
       <c r="AZ7" s="52">
         <f ca="1">AY7+1</f>
-        <v>45399</v>
+        <v>45405</v>
       </c>
       <c r="BA7" s="52">
         <f t="shared" ref="BA7:BE7" ca="1" si="1">AZ7+1</f>
-        <v>45400</v>
+        <v>45406</v>
       </c>
       <c r="BB7" s="52">
         <f t="shared" ca="1" si="1"/>
-        <v>45401</v>
+        <v>45407</v>
       </c>
       <c r="BC7" s="52">
         <f t="shared" ca="1" si="1"/>
-        <v>45402</v>
+        <v>45408</v>
       </c>
       <c r="BD7" s="52">
         <f t="shared" ca="1" si="1"/>
-        <v>45403</v>
+        <v>45409</v>
       </c>
       <c r="BE7" s="53">
         <f t="shared" ca="1" si="1"/>
-        <v>45404</v>
+        <v>45410</v>
       </c>
       <c r="BF7" s="52">
         <f ca="1">BE7+1</f>
-        <v>45405</v>
+        <v>45411</v>
       </c>
       <c r="BG7" s="52">
         <f ca="1">BF7+1</f>
-        <v>45406</v>
+        <v>45412</v>
       </c>
       <c r="BH7" s="52">
         <f t="shared" ref="BH7:BL7" ca="1" si="2">BG7+1</f>
-        <v>45407</v>
+        <v>45413</v>
       </c>
       <c r="BI7" s="52">
         <f t="shared" ca="1" si="2"/>
-        <v>45408</v>
+        <v>45414</v>
       </c>
       <c r="BJ7" s="52">
         <f t="shared" ca="1" si="2"/>
-        <v>45409</v>
+        <v>45415</v>
       </c>
       <c r="BK7" s="52">
         <f t="shared" ca="1" si="2"/>
-        <v>45410</v>
+        <v>45416</v>
       </c>
       <c r="BL7" s="53">
         <f t="shared" ca="1" si="2"/>
-        <v>45411</v>
+        <v>45417</v>
       </c>
     </row>
-    <row r="8" spans="1:68" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:68" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="6"/>
       <c r="B8" s="27"/>
       <c r="C8" s="27"/>
@@ -2885,7 +3057,7 @@
       <c r="BK8" s="55"/>
       <c r="BL8" s="58"/>
     </row>
-    <row r="9" spans="1:68" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:68" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="6"/>
       <c r="B9" s="48" t="s">
         <v>2</v>
@@ -2908,230 +3080,230 @@
       <c r="H9" s="41"/>
       <c r="I9" s="47" t="str">
         <f t="shared" ref="I9:BL9" ca="1" si="3">LEFT(TEXT(I7,"ddd"),1)</f>
-        <v>T</v>
+        <v>m</v>
       </c>
       <c r="J9" s="47" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>W</v>
+        <v>d</v>
       </c>
       <c r="K9" s="47" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>T</v>
+        <v>w</v>
       </c>
       <c r="L9" s="47" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>F</v>
+        <v>d</v>
       </c>
       <c r="M9" s="47" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>S</v>
+        <v>v</v>
       </c>
       <c r="N9" s="47" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>S</v>
+        <v>z</v>
       </c>
       <c r="O9" s="47" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>M</v>
+        <v>z</v>
       </c>
       <c r="P9" s="47" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>T</v>
+        <v>m</v>
       </c>
       <c r="Q9" s="47" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>W</v>
+        <v>d</v>
       </c>
       <c r="R9" s="47" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>T</v>
+        <v>w</v>
       </c>
       <c r="S9" s="47" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>F</v>
+        <v>d</v>
       </c>
       <c r="T9" s="47" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>S</v>
+        <v>v</v>
       </c>
       <c r="U9" s="47" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>S</v>
+        <v>z</v>
       </c>
       <c r="V9" s="47" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>M</v>
+        <v>z</v>
       </c>
       <c r="W9" s="47" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>T</v>
+        <v>m</v>
       </c>
       <c r="X9" s="47" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>W</v>
+        <v>d</v>
       </c>
       <c r="Y9" s="47" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>T</v>
+        <v>w</v>
       </c>
       <c r="Z9" s="47" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>F</v>
+        <v>d</v>
       </c>
       <c r="AA9" s="47" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>S</v>
+        <v>v</v>
       </c>
       <c r="AB9" s="47" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>S</v>
+        <v>z</v>
       </c>
       <c r="AC9" s="47" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>M</v>
+        <v>z</v>
       </c>
       <c r="AD9" s="47" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>T</v>
+        <v>m</v>
       </c>
       <c r="AE9" s="47" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>W</v>
+        <v>d</v>
       </c>
       <c r="AF9" s="47" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>T</v>
+        <v>w</v>
       </c>
       <c r="AG9" s="47" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>F</v>
+        <v>d</v>
       </c>
       <c r="AH9" s="47" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>S</v>
+        <v>v</v>
       </c>
       <c r="AI9" s="47" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>S</v>
+        <v>z</v>
       </c>
       <c r="AJ9" s="47" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>M</v>
+        <v>z</v>
       </c>
       <c r="AK9" s="47" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>T</v>
+        <v>m</v>
       </c>
       <c r="AL9" s="47" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>W</v>
+        <v>d</v>
       </c>
       <c r="AM9" s="47" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>T</v>
+        <v>w</v>
       </c>
       <c r="AN9" s="47" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>F</v>
+        <v>d</v>
       </c>
       <c r="AO9" s="47" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>S</v>
+        <v>v</v>
       </c>
       <c r="AP9" s="47" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>S</v>
+        <v>z</v>
       </c>
       <c r="AQ9" s="47" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>M</v>
+        <v>z</v>
       </c>
       <c r="AR9" s="47" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>T</v>
+        <v>m</v>
       </c>
       <c r="AS9" s="47" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>W</v>
+        <v>d</v>
       </c>
       <c r="AT9" s="47" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>T</v>
+        <v>w</v>
       </c>
       <c r="AU9" s="47" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>F</v>
+        <v>d</v>
       </c>
       <c r="AV9" s="47" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>S</v>
+        <v>v</v>
       </c>
       <c r="AW9" s="47" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>S</v>
+        <v>z</v>
       </c>
       <c r="AX9" s="47" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>M</v>
+        <v>z</v>
       </c>
       <c r="AY9" s="47" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>T</v>
+        <v>m</v>
       </c>
       <c r="AZ9" s="47" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>W</v>
+        <v>d</v>
       </c>
       <c r="BA9" s="47" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>T</v>
+        <v>w</v>
       </c>
       <c r="BB9" s="47" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>F</v>
+        <v>d</v>
       </c>
       <c r="BC9" s="47" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>S</v>
+        <v>v</v>
       </c>
       <c r="BD9" s="47" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>S</v>
+        <v>z</v>
       </c>
       <c r="BE9" s="47" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>M</v>
+        <v>z</v>
       </c>
       <c r="BF9" s="47" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>T</v>
+        <v>m</v>
       </c>
       <c r="BG9" s="47" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>W</v>
+        <v>d</v>
       </c>
       <c r="BH9" s="47" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>T</v>
+        <v>w</v>
       </c>
       <c r="BI9" s="47" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>F</v>
+        <v>d</v>
       </c>
       <c r="BJ9" s="47" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>S</v>
+        <v>v</v>
       </c>
       <c r="BK9" s="47" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>S</v>
+        <v>z</v>
       </c>
       <c r="BL9" s="47" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>M</v>
+        <v>z</v>
       </c>
     </row>
-    <row r="10" spans="1:68" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:68" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B10" s="11"/>
       <c r="C10" s="8"/>
       <c r="D10" s="7"/>
@@ -3195,7 +3367,7 @@
       <c r="BK10" s="13"/>
       <c r="BL10" s="13"/>
     </row>
-    <row r="11" spans="1:68" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:68" s="1" customFormat="1" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="6"/>
       <c r="B11" s="60" t="s">
         <v>16</v>
@@ -3432,7 +3604,7 @@
       </c>
       <c r="BP11" s="14"/>
     </row>
-    <row r="12" spans="1:68" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:68" s="1" customFormat="1" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="6"/>
       <c r="B12" s="19" t="s">
         <v>17</v>
@@ -3446,7 +3618,7 @@
       </c>
       <c r="F12" s="17">
         <f ca="1">TODAY()</f>
-        <v>45356</v>
+        <v>45358</v>
       </c>
       <c r="G12" s="18">
         <v>11</v>
@@ -3480,21 +3652,21 @@
         <f t="shared" ca="1" si="4"/>
         <v>2</v>
       </c>
-      <c r="P12" s="12">
+      <c r="P12" s="12" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>2</v>
-      </c>
-      <c r="Q12" s="12">
+        <v/>
+      </c>
+      <c r="Q12" s="12" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>2</v>
-      </c>
-      <c r="R12" s="12">
+        <v/>
+      </c>
+      <c r="R12" s="12" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>2</v>
-      </c>
-      <c r="S12" s="12">
+        <v/>
+      </c>
+      <c r="S12" s="12" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>2</v>
+        <v/>
       </c>
       <c r="T12" s="12" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -3677,10 +3849,10 @@
         <v/>
       </c>
     </row>
-    <row r="13" spans="1:68" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:68" s="1" customFormat="1" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="6"/>
       <c r="B13" s="19" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="C13" s="15" t="s">
         <v>5</v>
@@ -3778,29 +3950,29 @@
         <f t="shared" ca="1" si="5"/>
         <v/>
       </c>
-      <c r="AD13" s="12" t="str">
+      <c r="AD13" s="12">
         <f t="shared" ca="1" si="5"/>
-        <v/>
-      </c>
-      <c r="AE13" s="12" t="str">
+        <v>2</v>
+      </c>
+      <c r="AE13" s="12">
         <f t="shared" ca="1" si="5"/>
-        <v/>
-      </c>
-      <c r="AF13" s="12" t="str">
+        <v>2</v>
+      </c>
+      <c r="AF13" s="12">
         <f t="shared" ca="1" si="5"/>
-        <v/>
-      </c>
-      <c r="AG13" s="12" t="str">
+        <v>2</v>
+      </c>
+      <c r="AG13" s="12">
         <f t="shared" ca="1" si="5"/>
-        <v/>
-      </c>
-      <c r="AH13" s="12" t="str">
+        <v>2</v>
+      </c>
+      <c r="AH13" s="12">
         <f t="shared" ca="1" si="5"/>
-        <v/>
-      </c>
-      <c r="AI13" s="12" t="str">
+        <v>2</v>
+      </c>
+      <c r="AI13" s="12">
         <f t="shared" ca="1" si="5"/>
-        <v/>
+        <v>2</v>
       </c>
       <c r="AJ13" s="12">
         <f t="shared" ca="1" si="5"/>
@@ -3834,29 +4006,29 @@
         <f t="shared" ca="1" si="6"/>
         <v>2</v>
       </c>
-      <c r="AR13" s="12">
+      <c r="AR13" s="12" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>2</v>
-      </c>
-      <c r="AS13" s="12">
+        <v/>
+      </c>
+      <c r="AS13" s="12" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>2</v>
-      </c>
-      <c r="AT13" s="12">
+        <v/>
+      </c>
+      <c r="AT13" s="12" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>2</v>
-      </c>
-      <c r="AU13" s="12">
+        <v/>
+      </c>
+      <c r="AU13" s="12" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>2</v>
-      </c>
-      <c r="AV13" s="12">
+        <v/>
+      </c>
+      <c r="AV13" s="12" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>2</v>
-      </c>
-      <c r="AW13" s="12">
+        <v/>
+      </c>
+      <c r="AW13" s="12" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>2</v>
+        <v/>
       </c>
       <c r="AX13" s="12" t="str">
         <f t="shared" ca="1" si="6"/>
@@ -3919,7 +4091,7 @@
         <v/>
       </c>
     </row>
-    <row r="14" spans="1:68" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:68" s="1" customFormat="1" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="5"/>
       <c r="B14" s="19" t="s">
         <v>18</v>
@@ -4020,29 +4192,29 @@
         <f t="shared" ref="AC14:AL23" ca="1" si="11">IF(AND($C14="Doel",AC$7&gt;=$F14,AC$7&lt;=$F14+$G14-1),2,IF(AND($C14="Mijlpaal",AC$7&gt;=$F14,AC$7&lt;=$F14+$G14-1),1,""))</f>
         <v/>
       </c>
-      <c r="AD14" s="12" t="str">
+      <c r="AD14" s="12">
         <f t="shared" ca="1" si="11"/>
-        <v/>
-      </c>
-      <c r="AE14" s="12" t="str">
+        <v>2</v>
+      </c>
+      <c r="AE14" s="12">
         <f t="shared" ca="1" si="11"/>
-        <v/>
-      </c>
-      <c r="AF14" s="12" t="str">
+        <v>2</v>
+      </c>
+      <c r="AF14" s="12">
         <f t="shared" ca="1" si="11"/>
-        <v/>
-      </c>
-      <c r="AG14" s="12" t="str">
+        <v>2</v>
+      </c>
+      <c r="AG14" s="12">
         <f t="shared" ca="1" si="11"/>
-        <v/>
-      </c>
-      <c r="AH14" s="12" t="str">
+        <v>2</v>
+      </c>
+      <c r="AH14" s="12">
         <f t="shared" ca="1" si="11"/>
-        <v/>
-      </c>
-      <c r="AI14" s="12" t="str">
+        <v>2</v>
+      </c>
+      <c r="AI14" s="12">
         <f t="shared" ca="1" si="11"/>
-        <v/>
+        <v>2</v>
       </c>
       <c r="AJ14" s="12">
         <f t="shared" ca="1" si="11"/>
@@ -4076,29 +4248,29 @@
         <f t="shared" ca="1" si="12"/>
         <v>2</v>
       </c>
-      <c r="AR14" s="12">
+      <c r="AR14" s="12" t="str">
         <f t="shared" ca="1" si="12"/>
-        <v>2</v>
-      </c>
-      <c r="AS14" s="12">
+        <v/>
+      </c>
+      <c r="AS14" s="12" t="str">
         <f t="shared" ca="1" si="12"/>
-        <v>2</v>
-      </c>
-      <c r="AT14" s="12">
+        <v/>
+      </c>
+      <c r="AT14" s="12" t="str">
         <f t="shared" ca="1" si="12"/>
-        <v>2</v>
-      </c>
-      <c r="AU14" s="12">
+        <v/>
+      </c>
+      <c r="AU14" s="12" t="str">
         <f t="shared" ca="1" si="12"/>
-        <v>2</v>
-      </c>
-      <c r="AV14" s="12">
+        <v/>
+      </c>
+      <c r="AV14" s="12" t="str">
         <f t="shared" ca="1" si="12"/>
-        <v>2</v>
-      </c>
-      <c r="AW14" s="12">
+        <v/>
+      </c>
+      <c r="AW14" s="12" t="str">
         <f t="shared" ref="AW14:BF23" ca="1" si="13">IF(AND($C14="Doel",AW$7&gt;=$F14,AW$7&lt;=$F14+$G14-1),2,IF(AND($C14="Mijlpaal",AW$7&gt;=$F14,AW$7&lt;=$F14+$G14-1),1,""))</f>
-        <v>2</v>
+        <v/>
       </c>
       <c r="AX14" s="12" t="str">
         <f t="shared" ca="1" si="13"/>
@@ -4161,7 +4333,7 @@
         <v/>
       </c>
     </row>
-    <row r="15" spans="1:68" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:68" s="1" customFormat="1" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="5"/>
       <c r="B15" s="19" t="s">
         <v>19</v>
@@ -4262,29 +4434,29 @@
         <f t="shared" ca="1" si="11"/>
         <v/>
       </c>
-      <c r="AD15" s="12" t="str">
+      <c r="AD15" s="12">
         <f t="shared" ca="1" si="11"/>
-        <v/>
-      </c>
-      <c r="AE15" s="12" t="str">
+        <v>2</v>
+      </c>
+      <c r="AE15" s="12">
         <f t="shared" ca="1" si="11"/>
-        <v/>
-      </c>
-      <c r="AF15" s="12" t="str">
+        <v>2</v>
+      </c>
+      <c r="AF15" s="12">
         <f t="shared" ca="1" si="11"/>
-        <v/>
-      </c>
-      <c r="AG15" s="12" t="str">
+        <v>2</v>
+      </c>
+      <c r="AG15" s="12">
         <f t="shared" ca="1" si="11"/>
-        <v/>
-      </c>
-      <c r="AH15" s="12" t="str">
+        <v>2</v>
+      </c>
+      <c r="AH15" s="12">
         <f t="shared" ca="1" si="11"/>
-        <v/>
-      </c>
-      <c r="AI15" s="12" t="str">
+        <v>2</v>
+      </c>
+      <c r="AI15" s="12">
         <f t="shared" ca="1" si="11"/>
-        <v/>
+        <v>2</v>
       </c>
       <c r="AJ15" s="12">
         <f t="shared" ca="1" si="11"/>
@@ -4318,29 +4490,29 @@
         <f t="shared" ca="1" si="12"/>
         <v>2</v>
       </c>
-      <c r="AR15" s="12">
+      <c r="AR15" s="12" t="str">
         <f t="shared" ca="1" si="12"/>
-        <v>2</v>
-      </c>
-      <c r="AS15" s="12">
+        <v/>
+      </c>
+      <c r="AS15" s="12" t="str">
         <f t="shared" ca="1" si="12"/>
-        <v>2</v>
-      </c>
-      <c r="AT15" s="12">
+        <v/>
+      </c>
+      <c r="AT15" s="12" t="str">
         <f t="shared" ca="1" si="12"/>
-        <v>2</v>
-      </c>
-      <c r="AU15" s="12">
+        <v/>
+      </c>
+      <c r="AU15" s="12" t="str">
         <f t="shared" ca="1" si="12"/>
-        <v>2</v>
-      </c>
-      <c r="AV15" s="12">
+        <v/>
+      </c>
+      <c r="AV15" s="12" t="str">
         <f t="shared" ca="1" si="12"/>
-        <v>2</v>
-      </c>
-      <c r="AW15" s="12">
+        <v/>
+      </c>
+      <c r="AW15" s="12" t="str">
         <f t="shared" ca="1" si="13"/>
-        <v>2</v>
+        <v/>
       </c>
       <c r="AX15" s="12" t="str">
         <f t="shared" ca="1" si="13"/>
@@ -4403,7 +4575,7 @@
         <v/>
       </c>
     </row>
-    <row r="16" spans="1:68" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:68" s="1" customFormat="1" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="5"/>
       <c r="B16" s="19" t="s">
         <v>20</v>
@@ -4504,57 +4676,57 @@
         <f t="shared" ca="1" si="11"/>
         <v/>
       </c>
-      <c r="AD16" s="12" t="str">
+      <c r="AD16" s="12">
         <f t="shared" ca="1" si="11"/>
-        <v/>
-      </c>
-      <c r="AE16" s="12" t="str">
+        <v>2</v>
+      </c>
+      <c r="AE16" s="12">
         <f t="shared" ca="1" si="11"/>
-        <v/>
-      </c>
-      <c r="AF16" s="12" t="str">
+        <v>2</v>
+      </c>
+      <c r="AF16" s="12">
         <f t="shared" ca="1" si="11"/>
-        <v/>
-      </c>
-      <c r="AG16" s="12" t="str">
+        <v>2</v>
+      </c>
+      <c r="AG16" s="12">
         <f t="shared" ca="1" si="11"/>
-        <v/>
-      </c>
-      <c r="AH16" s="12" t="str">
+        <v>2</v>
+      </c>
+      <c r="AH16" s="12">
         <f t="shared" ca="1" si="11"/>
-        <v/>
-      </c>
-      <c r="AI16" s="12" t="str">
+        <v>2</v>
+      </c>
+      <c r="AI16" s="12">
         <f t="shared" ca="1" si="11"/>
-        <v/>
+        <v>2</v>
       </c>
       <c r="AJ16" s="12">
         <f t="shared" ca="1" si="11"/>
         <v>2</v>
       </c>
-      <c r="AK16" s="12">
+      <c r="AK16" s="12" t="str">
         <f t="shared" ca="1" si="11"/>
-        <v>2</v>
-      </c>
-      <c r="AL16" s="12">
+        <v/>
+      </c>
+      <c r="AL16" s="12" t="str">
         <f t="shared" ca="1" si="11"/>
-        <v>2</v>
-      </c>
-      <c r="AM16" s="12">
+        <v/>
+      </c>
+      <c r="AM16" s="12" t="str">
         <f t="shared" ca="1" si="12"/>
-        <v>2</v>
-      </c>
-      <c r="AN16" s="12">
+        <v/>
+      </c>
+      <c r="AN16" s="12" t="str">
         <f t="shared" ca="1" si="12"/>
-        <v>2</v>
-      </c>
-      <c r="AO16" s="12">
+        <v/>
+      </c>
+      <c r="AO16" s="12" t="str">
         <f t="shared" ca="1" si="12"/>
-        <v>2</v>
-      </c>
-      <c r="AP16" s="12">
+        <v/>
+      </c>
+      <c r="AP16" s="12" t="str">
         <f t="shared" ca="1" si="12"/>
-        <v>2</v>
+        <v/>
       </c>
       <c r="AQ16" s="12" t="str">
         <f t="shared" ca="1" si="12"/>
@@ -4645,10 +4817,10 @@
         <v/>
       </c>
     </row>
-    <row r="17" spans="1:64" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:64" s="1" customFormat="1" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="6"/>
       <c r="B17" s="19" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="C17" s="15" t="s">
         <v>5</v>
@@ -4718,29 +4890,29 @@
         <f t="shared" ca="1" si="10"/>
         <v/>
       </c>
-      <c r="W17" s="12" t="str">
+      <c r="W17" s="12">
         <f t="shared" ca="1" si="10"/>
-        <v/>
-      </c>
-      <c r="X17" s="12" t="str">
+        <v>2</v>
+      </c>
+      <c r="X17" s="12">
         <f t="shared" ca="1" si="10"/>
-        <v/>
-      </c>
-      <c r="Y17" s="12" t="str">
+        <v>2</v>
+      </c>
+      <c r="Y17" s="12">
         <f t="shared" ca="1" si="10"/>
-        <v/>
-      </c>
-      <c r="Z17" s="12" t="str">
+        <v>2</v>
+      </c>
+      <c r="Z17" s="12">
         <f t="shared" ca="1" si="10"/>
-        <v/>
-      </c>
-      <c r="AA17" s="12" t="str">
+        <v>2</v>
+      </c>
+      <c r="AA17" s="12">
         <f t="shared" ca="1" si="10"/>
-        <v/>
-      </c>
-      <c r="AB17" s="12" t="str">
+        <v>2</v>
+      </c>
+      <c r="AB17" s="12">
         <f t="shared" ca="1" si="10"/>
-        <v/>
+        <v>2</v>
       </c>
       <c r="AC17" s="12">
         <f t="shared" ca="1" si="11"/>
@@ -4774,29 +4946,29 @@
         <f t="shared" ca="1" si="11"/>
         <v>2</v>
       </c>
-      <c r="AK17" s="12">
+      <c r="AK17" s="12" t="str">
         <f t="shared" ca="1" si="11"/>
-        <v>2</v>
-      </c>
-      <c r="AL17" s="12">
+        <v/>
+      </c>
+      <c r="AL17" s="12" t="str">
         <f t="shared" ca="1" si="11"/>
-        <v>2</v>
-      </c>
-      <c r="AM17" s="12">
+        <v/>
+      </c>
+      <c r="AM17" s="12" t="str">
         <f t="shared" ca="1" si="12"/>
-        <v>2</v>
-      </c>
-      <c r="AN17" s="12">
+        <v/>
+      </c>
+      <c r="AN17" s="12" t="str">
         <f t="shared" ca="1" si="12"/>
-        <v>2</v>
-      </c>
-      <c r="AO17" s="12">
+        <v/>
+      </c>
+      <c r="AO17" s="12" t="str">
         <f t="shared" ca="1" si="12"/>
-        <v>2</v>
-      </c>
-      <c r="AP17" s="12">
+        <v/>
+      </c>
+      <c r="AP17" s="12" t="str">
         <f t="shared" ca="1" si="12"/>
-        <v>2</v>
+        <v/>
       </c>
       <c r="AQ17" s="12" t="str">
         <f t="shared" ca="1" si="12"/>
@@ -4887,7 +5059,7 @@
         <v/>
       </c>
     </row>
-    <row r="18" spans="1:64" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:64" s="1" customFormat="1" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="5"/>
       <c r="B18" s="19" t="s">
         <v>21</v>
@@ -5044,29 +5216,29 @@
         <f t="shared" ca="1" si="12"/>
         <v/>
       </c>
-      <c r="AR18" s="12" t="str">
+      <c r="AR18" s="12">
         <f t="shared" ca="1" si="12"/>
-        <v/>
-      </c>
-      <c r="AS18" s="12" t="str">
+        <v>2</v>
+      </c>
+      <c r="AS18" s="12">
         <f t="shared" ca="1" si="12"/>
-        <v/>
-      </c>
-      <c r="AT18" s="12" t="str">
+        <v>2</v>
+      </c>
+      <c r="AT18" s="12">
         <f t="shared" ca="1" si="12"/>
-        <v/>
-      </c>
-      <c r="AU18" s="12" t="str">
+        <v>2</v>
+      </c>
+      <c r="AU18" s="12">
         <f t="shared" ca="1" si="12"/>
-        <v/>
-      </c>
-      <c r="AV18" s="12" t="str">
+        <v>2</v>
+      </c>
+      <c r="AV18" s="12">
         <f t="shared" ca="1" si="12"/>
-        <v/>
-      </c>
-      <c r="AW18" s="12" t="str">
+        <v>2</v>
+      </c>
+      <c r="AW18" s="12">
         <f t="shared" ca="1" si="13"/>
-        <v/>
+        <v>2</v>
       </c>
       <c r="AX18" s="12">
         <f t="shared" ca="1" si="13"/>
@@ -5129,7 +5301,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:64" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:64" s="1" customFormat="1" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="5"/>
       <c r="B19" s="60" t="s">
         <v>22</v>
@@ -5365,7 +5537,7 @@
         <v/>
       </c>
     </row>
-    <row r="20" spans="1:64" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:64" s="1" customFormat="1" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="5"/>
       <c r="B20" s="19" t="s">
         <v>28</v>
@@ -5461,7 +5633,7 @@
       <c r="BK20" s="12"/>
       <c r="BL20" s="12"/>
     </row>
-    <row r="21" spans="1:64" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:64" s="1" customFormat="1" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="5"/>
       <c r="B21" s="19" t="s">
         <v>29</v>
@@ -5472,7 +5644,9 @@
       <c r="D21" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="E21" s="16"/>
+      <c r="E21" s="16" t="s">
+        <v>58</v>
+      </c>
       <c r="F21" s="17">
         <v>45337</v>
       </c>
@@ -5705,7 +5879,7 @@
         <v/>
       </c>
     </row>
-    <row r="22" spans="1:64" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:64" s="1" customFormat="1" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="5"/>
       <c r="B22" s="19" t="s">
         <v>30</v>
@@ -5717,7 +5891,7 @@
         <v>24</v>
       </c>
       <c r="E22" s="16">
-        <v>0.7</v>
+        <v>0.72</v>
       </c>
       <c r="F22" s="17">
         <v>45337</v>
@@ -5951,10 +6125,10 @@
         <v/>
       </c>
     </row>
-    <row r="23" spans="1:64" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:64" s="1" customFormat="1" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="5"/>
       <c r="B23" s="59" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C23" s="15"/>
       <c r="D23" s="15"/>
@@ -6187,7 +6361,7 @@
         <v/>
       </c>
     </row>
-    <row r="24" spans="1:64" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:64" s="1" customFormat="1" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="5"/>
       <c r="B24" s="19" t="s">
         <v>31</v>
@@ -6433,7 +6607,7 @@
         <v/>
       </c>
     </row>
-    <row r="25" spans="1:64" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:64" s="1" customFormat="1" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="5"/>
       <c r="B25" s="19" t="s">
         <v>32</v>
@@ -6480,29 +6654,29 @@
         <f t="shared" ca="1" si="15"/>
         <v>2</v>
       </c>
-      <c r="P25" s="12">
+      <c r="P25" s="12" t="str">
         <f t="shared" ca="1" si="15"/>
-        <v>2</v>
-      </c>
-      <c r="Q25" s="12">
+        <v/>
+      </c>
+      <c r="Q25" s="12" t="str">
         <f t="shared" ca="1" si="15"/>
-        <v>2</v>
-      </c>
-      <c r="R25" s="12">
+        <v/>
+      </c>
+      <c r="R25" s="12" t="str">
         <f t="shared" ca="1" si="15"/>
-        <v>2</v>
-      </c>
-      <c r="S25" s="12">
+        <v/>
+      </c>
+      <c r="S25" s="12" t="str">
         <f t="shared" ca="1" si="16"/>
-        <v>2</v>
-      </c>
-      <c r="T25" s="12">
+        <v/>
+      </c>
+      <c r="T25" s="12" t="str">
         <f t="shared" ca="1" si="16"/>
-        <v>2</v>
-      </c>
-      <c r="U25" s="12">
+        <v/>
+      </c>
+      <c r="U25" s="12" t="str">
         <f t="shared" ca="1" si="16"/>
-        <v>2</v>
+        <v/>
       </c>
       <c r="V25" s="12" t="str">
         <f t="shared" ca="1" si="16"/>
@@ -6677,7 +6851,7 @@
         <v/>
       </c>
     </row>
-    <row r="26" spans="1:64" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:64" s="1" customFormat="1" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="5"/>
       <c r="B26" s="19" t="s">
         <v>33</v>
@@ -6688,7 +6862,9 @@
       <c r="D26" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="E26" s="16"/>
+      <c r="E26" s="16">
+        <v>1</v>
+      </c>
       <c r="F26" s="17">
         <v>45344</v>
       </c>
@@ -6696,13 +6872,13 @@
         <v>14</v>
       </c>
       <c r="H26" s="15"/>
-      <c r="I26" s="12">
+      <c r="I26" s="12" t="str">
         <f t="shared" ca="1" si="15"/>
-        <v>1</v>
-      </c>
-      <c r="J26" s="12">
+        <v/>
+      </c>
+      <c r="J26" s="12" t="str">
         <f t="shared" ca="1" si="15"/>
-        <v>1</v>
+        <v/>
       </c>
       <c r="K26" s="12" t="str">
         <f t="shared" ca="1" si="15"/>
@@ -6921,7 +7097,7 @@
         <v/>
       </c>
     </row>
-    <row r="27" spans="1:64" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:64" s="1" customFormat="1" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="5"/>
       <c r="B27" s="19" t="s">
         <v>35</v>
@@ -7167,7 +7343,7 @@
         <v/>
       </c>
     </row>
-    <row r="28" spans="1:64" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:64" s="1" customFormat="1" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="5"/>
       <c r="B28" s="19" t="s">
         <v>37</v>
@@ -7178,7 +7354,9 @@
       <c r="D28" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="E28" s="16"/>
+      <c r="E28" s="16">
+        <v>0.75</v>
+      </c>
       <c r="F28" s="17">
         <v>45354</v>
       </c>
@@ -7411,7 +7589,7 @@
         <v/>
       </c>
     </row>
-    <row r="29" spans="1:64" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:64" s="1" customFormat="1" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="5"/>
       <c r="B29" s="19" t="s">
         <v>38</v>
@@ -7423,7 +7601,7 @@
         <v>34</v>
       </c>
       <c r="E29" s="16">
-        <v>0.35</v>
+        <v>0.6</v>
       </c>
       <c r="F29" s="17">
         <v>45351</v>
@@ -7657,10 +7835,10 @@
         <v/>
       </c>
     </row>
-    <row r="30" spans="1:64" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:64" s="1" customFormat="1" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="5"/>
       <c r="B30" s="59" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C30" s="15"/>
       <c r="D30" s="15"/>
@@ -7893,7 +8071,7 @@
         <v/>
       </c>
     </row>
-    <row r="31" spans="1:64" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:64" s="1" customFormat="1" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="5"/>
       <c r="B31" s="19" t="s">
         <v>39</v>
@@ -7969,10 +8147,10 @@
       <c r="BK31" s="12"/>
       <c r="BL31" s="12"/>
     </row>
-    <row r="32" spans="1:64" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:64" s="1" customFormat="1" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="5"/>
       <c r="B32" s="19" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C32" s="15" t="s">
         <v>7</v>
@@ -7980,7 +8158,9 @@
       <c r="D32" s="15" t="s">
         <v>40</v>
       </c>
-      <c r="E32" s="16"/>
+      <c r="E32" s="16">
+        <v>0.25</v>
+      </c>
       <c r="F32" s="17">
         <v>45358</v>
       </c>
@@ -8213,10 +8393,10 @@
         <v/>
       </c>
     </row>
-    <row r="33" spans="1:65" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:65" s="1" customFormat="1" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="5"/>
       <c r="B33" s="19" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C33" s="15" t="s">
         <v>8</v>
@@ -8289,16 +8469,16 @@
       <c r="BK33" s="12"/>
       <c r="BL33" s="12"/>
     </row>
-    <row r="34" spans="1:65" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:65" s="1" customFormat="1" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="5"/>
       <c r="B34" s="19" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C34" s="15" t="s">
         <v>8</v>
       </c>
       <c r="D34" s="15" t="s">
-        <v>40</v>
+        <v>57</v>
       </c>
       <c r="E34" s="16"/>
       <c r="F34" s="17">
@@ -8365,16 +8545,16 @@
       <c r="BK34" s="12"/>
       <c r="BL34" s="12"/>
     </row>
-    <row r="35" spans="1:65" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:65" s="1" customFormat="1" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="5"/>
       <c r="B35" s="19" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C35" s="15" t="s">
         <v>8</v>
       </c>
       <c r="D35" s="15" t="s">
-        <v>40</v>
+        <v>57</v>
       </c>
       <c r="E35" s="16"/>
       <c r="F35" s="17">
@@ -8441,16 +8621,16 @@
       <c r="BK35" s="12"/>
       <c r="BL35" s="12"/>
     </row>
-    <row r="36" spans="1:65" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:65" s="1" customFormat="1" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="5"/>
       <c r="B36" s="19" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C36" s="15" t="s">
         <v>6</v>
       </c>
       <c r="D36" s="15" t="s">
-        <v>34</v>
+        <v>51</v>
       </c>
       <c r="E36" s="16">
         <v>0.5</v>
@@ -8519,10 +8699,10 @@
       <c r="BK36" s="12"/>
       <c r="BL36" s="12"/>
     </row>
-    <row r="37" spans="1:65" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:65" s="1" customFormat="1" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="5"/>
       <c r="B37" s="19" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C37" s="15" t="s">
         <v>27</v>
@@ -8538,13 +8718,13 @@
         <v>18</v>
       </c>
       <c r="H37" s="15"/>
-      <c r="I37" s="12" t="str">
-        <f t="shared" ref="I37:R39" ca="1" si="23">IF(AND($C37="Doel",I$7&gt;=$F37,I$7&lt;=$F37+$G37-1),2,IF(AND($C37="Mijlpaal",I$7&gt;=$F37,I$7&lt;=$F37+$G37-1),1,""))</f>
-        <v/>
-      </c>
-      <c r="J37" s="12" t="str">
+      <c r="I37" s="12">
+        <f t="shared" ref="I37:R38" ca="1" si="23">IF(AND($C37="Doel",I$7&gt;=$F37,I$7&lt;=$F37+$G37-1),2,IF(AND($C37="Mijlpaal",I$7&gt;=$F37,I$7&lt;=$F37+$G37-1),1,""))</f>
+        <v>1</v>
+      </c>
+      <c r="J37" s="12">
         <f t="shared" ca="1" si="23"/>
-        <v/>
+        <v>1</v>
       </c>
       <c r="K37" s="12">
         <f t="shared" ca="1" si="23"/>
@@ -8579,7 +8759,7 @@
         <v>1</v>
       </c>
       <c r="S37" s="12">
-        <f t="shared" ref="S37:AB39" ca="1" si="24">IF(AND($C37="Doel",S$7&gt;=$F37,S$7&lt;=$F37+$G37-1),2,IF(AND($C37="Mijlpaal",S$7&gt;=$F37,S$7&lt;=$F37+$G37-1),1,""))</f>
+        <f t="shared" ref="S37:AB38" ca="1" si="24">IF(AND($C37="Doel",S$7&gt;=$F37,S$7&lt;=$F37+$G37-1),2,IF(AND($C37="Mijlpaal",S$7&gt;=$F37,S$7&lt;=$F37+$G37-1),1,""))</f>
         <v>1</v>
       </c>
       <c r="T37" s="12">
@@ -8594,32 +8774,32 @@
         <f t="shared" ca="1" si="24"/>
         <v>1</v>
       </c>
-      <c r="W37" s="12">
+      <c r="W37" s="12" t="str">
         <f t="shared" ca="1" si="24"/>
-        <v>1</v>
-      </c>
-      <c r="X37" s="12">
+        <v/>
+      </c>
+      <c r="X37" s="12" t="str">
         <f t="shared" ca="1" si="24"/>
-        <v>1</v>
-      </c>
-      <c r="Y37" s="12">
+        <v/>
+      </c>
+      <c r="Y37" s="12" t="str">
         <f t="shared" ca="1" si="24"/>
-        <v>1</v>
-      </c>
-      <c r="Z37" s="12">
+        <v/>
+      </c>
+      <c r="Z37" s="12" t="str">
         <f t="shared" ca="1" si="24"/>
-        <v>1</v>
-      </c>
-      <c r="AA37" s="12">
+        <v/>
+      </c>
+      <c r="AA37" s="12" t="str">
         <f t="shared" ca="1" si="24"/>
-        <v>1</v>
-      </c>
-      <c r="AB37" s="12">
+        <v/>
+      </c>
+      <c r="AB37" s="12" t="str">
         <f t="shared" ca="1" si="24"/>
-        <v>1</v>
+        <v/>
       </c>
       <c r="AC37" s="12" t="str">
-        <f t="shared" ref="AC37:AL39" ca="1" si="25">IF(AND($C37="Doel",AC$7&gt;=$F37,AC$7&lt;=$F37+$G37-1),2,IF(AND($C37="Mijlpaal",AC$7&gt;=$F37,AC$7&lt;=$F37+$G37-1),1,""))</f>
+        <f t="shared" ref="AC37:AL38" ca="1" si="25">IF(AND($C37="Doel",AC$7&gt;=$F37,AC$7&lt;=$F37+$G37-1),2,IF(AND($C37="Mijlpaal",AC$7&gt;=$F37,AC$7&lt;=$F37+$G37-1),1,""))</f>
         <v/>
       </c>
       <c r="AD37" s="12" t="str">
@@ -8659,7 +8839,7 @@
         <v/>
       </c>
       <c r="AM37" s="12" t="str">
-        <f t="shared" ref="AM37:AV39" ca="1" si="26">IF(AND($C37="Doel",AM$7&gt;=$F37,AM$7&lt;=$F37+$G37-1),2,IF(AND($C37="Mijlpaal",AM$7&gt;=$F37,AM$7&lt;=$F37+$G37-1),1,""))</f>
+        <f t="shared" ref="AM37:AV38" ca="1" si="26">IF(AND($C37="Doel",AM$7&gt;=$F37,AM$7&lt;=$F37+$G37-1),2,IF(AND($C37="Mijlpaal",AM$7&gt;=$F37,AM$7&lt;=$F37+$G37-1),1,""))</f>
         <v/>
       </c>
       <c r="AN37" s="12" t="str">
@@ -8699,7 +8879,7 @@
         <v/>
       </c>
       <c r="AW37" s="12" t="str">
-        <f t="shared" ref="AW37:BF39" ca="1" si="27">IF(AND($C37="Doel",AW$7&gt;=$F37,AW$7&lt;=$F37+$G37-1),2,IF(AND($C37="Mijlpaal",AW$7&gt;=$F37,AW$7&lt;=$F37+$G37-1),1,""))</f>
+        <f t="shared" ref="AW37:BF38" ca="1" si="27">IF(AND($C37="Doel",AW$7&gt;=$F37,AW$7&lt;=$F37+$G37-1),2,IF(AND($C37="Mijlpaal",AW$7&gt;=$F37,AW$7&lt;=$F37+$G37-1),1,""))</f>
         <v/>
       </c>
       <c r="AX37" s="12" t="str">
@@ -8739,7 +8919,7 @@
         <v/>
       </c>
       <c r="BG37" s="12" t="str">
-        <f t="shared" ref="BG37:BL39" ca="1" si="28">IF(AND($C37="Doel",BG$7&gt;=$F37,BG$7&lt;=$F37+$G37-1),2,IF(AND($C37="Mijlpaal",BG$7&gt;=$F37,BG$7&lt;=$F37+$G37-1),1,""))</f>
+        <f t="shared" ref="BG37:BL38" ca="1" si="28">IF(AND($C37="Doel",BG$7&gt;=$F37,BG$7&lt;=$F37+$G37-1),2,IF(AND($C37="Mijlpaal",BG$7&gt;=$F37,BG$7&lt;=$F37+$G37-1),1,""))</f>
         <v/>
       </c>
       <c r="BH37" s="12" t="str">
@@ -8763,10 +8943,10 @@
         <v/>
       </c>
     </row>
-    <row r="38" spans="1:65" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:65" s="1" customFormat="1" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" s="5"/>
       <c r="B38" s="59" t="s">
-        <v>53</v>
+        <v>66</v>
       </c>
       <c r="C38" s="15"/>
       <c r="D38" s="15"/>
@@ -8999,267 +9179,267 @@
         <v/>
       </c>
     </row>
-    <row r="39" spans="1:65" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:65" s="1" customFormat="1" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="5"/>
       <c r="B39" s="19" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="C39" s="15" t="s">
         <v>27</v>
       </c>
       <c r="D39" s="15" t="s">
-        <v>25</v>
+        <v>41</v>
       </c>
       <c r="E39" s="16"/>
       <c r="F39" s="17">
         <v>45379</v>
       </c>
       <c r="G39" s="18">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="H39" s="15"/>
       <c r="I39" s="12" t="str">
-        <f t="shared" ca="1" si="23"/>
+        <f t="shared" ref="I39:AN39" ca="1" si="29">IF(AND($C39="Doel",I$7&gt;=$F39,I$7&lt;=$F39+$G39-1),2,IF(AND($C39="Mijlpaal",I$7&gt;=$F39,I$7&lt;=$F39+$G39-1),1,""))</f>
         <v/>
       </c>
       <c r="J39" s="12" t="str">
-        <f t="shared" ca="1" si="23"/>
+        <f t="shared" ca="1" si="29"/>
         <v/>
       </c>
       <c r="K39" s="12" t="str">
-        <f t="shared" ca="1" si="23"/>
+        <f t="shared" ca="1" si="29"/>
         <v/>
       </c>
       <c r="L39" s="12" t="str">
-        <f t="shared" ca="1" si="23"/>
+        <f t="shared" ca="1" si="29"/>
         <v/>
       </c>
       <c r="M39" s="12" t="str">
-        <f t="shared" ca="1" si="23"/>
+        <f t="shared" ca="1" si="29"/>
         <v/>
       </c>
       <c r="N39" s="12" t="str">
-        <f t="shared" ca="1" si="23"/>
+        <f t="shared" ca="1" si="29"/>
         <v/>
       </c>
       <c r="O39" s="12" t="str">
-        <f t="shared" ca="1" si="23"/>
+        <f t="shared" ca="1" si="29"/>
         <v/>
       </c>
       <c r="P39" s="12" t="str">
-        <f t="shared" ca="1" si="23"/>
+        <f t="shared" ca="1" si="29"/>
         <v/>
       </c>
       <c r="Q39" s="12" t="str">
-        <f t="shared" ca="1" si="23"/>
+        <f t="shared" ca="1" si="29"/>
         <v/>
       </c>
       <c r="R39" s="12" t="str">
-        <f t="shared" ca="1" si="23"/>
+        <f t="shared" ca="1" si="29"/>
         <v/>
       </c>
       <c r="S39" s="12" t="str">
-        <f t="shared" ca="1" si="24"/>
+        <f t="shared" ca="1" si="29"/>
         <v/>
       </c>
       <c r="T39" s="12" t="str">
-        <f t="shared" ca="1" si="24"/>
+        <f t="shared" ca="1" si="29"/>
         <v/>
       </c>
       <c r="U39" s="12" t="str">
-        <f t="shared" ca="1" si="24"/>
+        <f t="shared" ca="1" si="29"/>
         <v/>
       </c>
       <c r="V39" s="12" t="str">
-        <f t="shared" ca="1" si="24"/>
+        <f t="shared" ca="1" si="29"/>
         <v/>
       </c>
       <c r="W39" s="12" t="str">
-        <f t="shared" ca="1" si="24"/>
+        <f t="shared" ca="1" si="29"/>
         <v/>
       </c>
       <c r="X39" s="12" t="str">
-        <f t="shared" ca="1" si="24"/>
+        <f t="shared" ca="1" si="29"/>
         <v/>
       </c>
       <c r="Y39" s="12" t="str">
-        <f t="shared" ca="1" si="24"/>
-        <v/>
-      </c>
-      <c r="Z39" s="12" t="str">
-        <f t="shared" ca="1" si="24"/>
-        <v/>
+        <f t="shared" ca="1" si="29"/>
+        <v/>
+      </c>
+      <c r="Z39" s="12">
+        <f t="shared" ca="1" si="29"/>
+        <v>1</v>
       </c>
       <c r="AA39" s="12" t="str">
-        <f t="shared" ca="1" si="24"/>
+        <f t="shared" ca="1" si="29"/>
         <v/>
       </c>
       <c r="AB39" s="12" t="str">
-        <f t="shared" ca="1" si="24"/>
+        <f t="shared" ca="1" si="29"/>
         <v/>
       </c>
       <c r="AC39" s="12" t="str">
-        <f t="shared" ca="1" si="25"/>
+        <f t="shared" ca="1" si="29"/>
         <v/>
       </c>
       <c r="AD39" s="12" t="str">
-        <f t="shared" ca="1" si="25"/>
+        <f t="shared" ca="1" si="29"/>
         <v/>
       </c>
       <c r="AE39" s="12" t="str">
-        <f t="shared" ca="1" si="25"/>
-        <v/>
-      </c>
-      <c r="AF39" s="12">
-        <f t="shared" ca="1" si="25"/>
-        <v>1</v>
-      </c>
-      <c r="AG39" s="12">
-        <f t="shared" ca="1" si="25"/>
-        <v>1</v>
-      </c>
-      <c r="AH39" s="12">
-        <f t="shared" ca="1" si="25"/>
-        <v>1</v>
-      </c>
-      <c r="AI39" s="12">
-        <f t="shared" ca="1" si="25"/>
-        <v>1</v>
-      </c>
-      <c r="AJ39" s="12">
-        <f t="shared" ca="1" si="25"/>
-        <v>1</v>
-      </c>
-      <c r="AK39" s="12">
-        <f t="shared" ca="1" si="25"/>
-        <v>1</v>
+        <f t="shared" ca="1" si="29"/>
+        <v/>
+      </c>
+      <c r="AF39" s="12" t="str">
+        <f t="shared" ca="1" si="29"/>
+        <v/>
+      </c>
+      <c r="AG39" s="12" t="str">
+        <f t="shared" ca="1" si="29"/>
+        <v/>
+      </c>
+      <c r="AH39" s="12" t="str">
+        <f t="shared" ca="1" si="29"/>
+        <v/>
+      </c>
+      <c r="AI39" s="12" t="str">
+        <f t="shared" ca="1" si="29"/>
+        <v/>
+      </c>
+      <c r="AJ39" s="12" t="str">
+        <f t="shared" ca="1" si="29"/>
+        <v/>
+      </c>
+      <c r="AK39" s="12" t="str">
+        <f t="shared" ca="1" si="29"/>
+        <v/>
       </c>
       <c r="AL39" s="12" t="str">
-        <f t="shared" ca="1" si="25"/>
+        <f t="shared" ca="1" si="29"/>
         <v/>
       </c>
       <c r="AM39" s="12" t="str">
-        <f t="shared" ca="1" si="26"/>
+        <f t="shared" ca="1" si="29"/>
         <v/>
       </c>
       <c r="AN39" s="12" t="str">
-        <f t="shared" ca="1" si="26"/>
+        <f t="shared" ca="1" si="29"/>
         <v/>
       </c>
       <c r="AO39" s="12" t="str">
-        <f t="shared" ca="1" si="26"/>
+        <f t="shared" ref="AO39:BL39" ca="1" si="30">IF(AND($C39="Doel",AO$7&gt;=$F39,AO$7&lt;=$F39+$G39-1),2,IF(AND($C39="Mijlpaal",AO$7&gt;=$F39,AO$7&lt;=$F39+$G39-1),1,""))</f>
         <v/>
       </c>
       <c r="AP39" s="12" t="str">
-        <f t="shared" ca="1" si="26"/>
+        <f t="shared" ca="1" si="30"/>
         <v/>
       </c>
       <c r="AQ39" s="12" t="str">
-        <f t="shared" ca="1" si="26"/>
+        <f t="shared" ca="1" si="30"/>
         <v/>
       </c>
       <c r="AR39" s="12" t="str">
-        <f t="shared" ca="1" si="26"/>
+        <f t="shared" ca="1" si="30"/>
         <v/>
       </c>
       <c r="AS39" s="12" t="str">
-        <f t="shared" ca="1" si="26"/>
+        <f t="shared" ca="1" si="30"/>
         <v/>
       </c>
       <c r="AT39" s="12" t="str">
-        <f t="shared" ca="1" si="26"/>
+        <f t="shared" ca="1" si="30"/>
         <v/>
       </c>
       <c r="AU39" s="12" t="str">
-        <f t="shared" ca="1" si="26"/>
+        <f t="shared" ca="1" si="30"/>
         <v/>
       </c>
       <c r="AV39" s="12" t="str">
-        <f t="shared" ca="1" si="26"/>
+        <f t="shared" ca="1" si="30"/>
         <v/>
       </c>
       <c r="AW39" s="12" t="str">
-        <f t="shared" ca="1" si="27"/>
+        <f t="shared" ca="1" si="30"/>
         <v/>
       </c>
       <c r="AX39" s="12" t="str">
-        <f t="shared" ca="1" si="27"/>
+        <f t="shared" ca="1" si="30"/>
         <v/>
       </c>
       <c r="AY39" s="12" t="str">
-        <f t="shared" ca="1" si="27"/>
+        <f t="shared" ca="1" si="30"/>
         <v/>
       </c>
       <c r="AZ39" s="12" t="str">
-        <f t="shared" ca="1" si="27"/>
+        <f t="shared" ca="1" si="30"/>
         <v/>
       </c>
       <c r="BA39" s="12" t="str">
-        <f t="shared" ca="1" si="27"/>
+        <f t="shared" ca="1" si="30"/>
         <v/>
       </c>
       <c r="BB39" s="12" t="str">
-        <f t="shared" ca="1" si="27"/>
+        <f t="shared" ca="1" si="30"/>
         <v/>
       </c>
       <c r="BC39" s="12" t="str">
-        <f t="shared" ca="1" si="27"/>
+        <f t="shared" ca="1" si="30"/>
         <v/>
       </c>
       <c r="BD39" s="12" t="str">
-        <f t="shared" ca="1" si="27"/>
+        <f t="shared" ca="1" si="30"/>
         <v/>
       </c>
       <c r="BE39" s="12" t="str">
-        <f t="shared" ca="1" si="27"/>
+        <f t="shared" ca="1" si="30"/>
         <v/>
       </c>
       <c r="BF39" s="12" t="str">
-        <f t="shared" ca="1" si="27"/>
+        <f t="shared" ca="1" si="30"/>
         <v/>
       </c>
       <c r="BG39" s="12" t="str">
-        <f t="shared" ca="1" si="28"/>
+        <f t="shared" ca="1" si="30"/>
         <v/>
       </c>
       <c r="BH39" s="12" t="str">
-        <f t="shared" ca="1" si="28"/>
+        <f t="shared" ca="1" si="30"/>
         <v/>
       </c>
       <c r="BI39" s="12" t="str">
-        <f t="shared" ca="1" si="28"/>
+        <f t="shared" ca="1" si="30"/>
         <v/>
       </c>
       <c r="BJ39" s="12" t="str">
-        <f t="shared" ca="1" si="28"/>
+        <f t="shared" ca="1" si="30"/>
         <v/>
       </c>
       <c r="BK39" s="12" t="str">
-        <f t="shared" ca="1" si="28"/>
+        <f t="shared" ca="1" si="30"/>
         <v/>
       </c>
       <c r="BL39" s="12" t="str">
-        <f t="shared" ca="1" si="28"/>
+        <f t="shared" ca="1" si="30"/>
         <v/>
       </c>
     </row>
-    <row r="40" spans="1:65" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:65" s="1" customFormat="1" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" s="5"/>
       <c r="B40" s="19" t="s">
-        <v>46</v>
+        <v>60</v>
       </c>
       <c r="C40" s="15" t="s">
-        <v>27</v>
+        <v>8</v>
       </c>
       <c r="D40" s="15" t="s">
-        <v>41</v>
+        <v>25</v>
       </c>
       <c r="E40" s="16"/>
       <c r="F40" s="17">
-        <v>45382</v>
+        <v>45379</v>
       </c>
       <c r="G40" s="18">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="H40" s="15"/>
       <c r="I40" s="12"/>
@@ -9319,16 +9499,24 @@
       <c r="BK40" s="12"/>
       <c r="BL40" s="12"/>
     </row>
-    <row r="41" spans="1:65" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:65" s="1" customFormat="1" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" s="5"/>
-      <c r="B41" s="59" t="s">
-        <v>59</v>
-      </c>
-      <c r="C41" s="15"/>
-      <c r="D41" s="15"/>
-      <c r="E41" s="16"/>
-      <c r="F41" s="17"/>
-      <c r="G41" s="18"/>
+      <c r="B41" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="C41" s="66" t="s">
+        <v>7</v>
+      </c>
+      <c r="D41" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="E41" s="67"/>
+      <c r="F41" s="68">
+        <v>45379</v>
+      </c>
+      <c r="G41" s="69">
+        <v>14</v>
+      </c>
       <c r="H41" s="15"/>
       <c r="I41" s="12"/>
       <c r="J41" s="12"/>
@@ -9387,24 +9575,16 @@
       <c r="BK41" s="12"/>
       <c r="BL41" s="12"/>
     </row>
-    <row r="42" spans="1:65" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:65" s="1" customFormat="1" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" s="5"/>
-      <c r="B42" s="19" t="s">
-        <v>45</v>
-      </c>
-      <c r="C42" s="15" t="s">
-        <v>5</v>
-      </c>
-      <c r="D42" s="15" t="s">
-        <v>36</v>
-      </c>
+      <c r="B42" s="59" t="s">
+        <v>67</v>
+      </c>
+      <c r="C42" s="15"/>
+      <c r="D42" s="15"/>
       <c r="E42" s="16"/>
-      <c r="F42" s="17">
-        <v>45383</v>
-      </c>
-      <c r="G42" s="18">
-        <v>14</v>
-      </c>
+      <c r="F42" s="17"/>
+      <c r="G42" s="18"/>
       <c r="H42" s="15"/>
       <c r="I42" s="12"/>
       <c r="J42" s="12"/>
@@ -9463,22 +9643,20 @@
       <c r="BK42" s="12"/>
       <c r="BL42" s="12"/>
     </row>
-    <row r="43" spans="1:65" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:65" s="1" customFormat="1" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A43" s="5"/>
       <c r="B43" s="19" t="s">
-        <v>54</v>
-      </c>
-      <c r="C43" s="15" t="s">
-        <v>5</v>
-      </c>
-      <c r="D43" s="15" t="s">
-        <v>55</v>
-      </c>
-      <c r="E43" s="16"/>
-      <c r="F43" s="17">
-        <v>45383</v>
-      </c>
-      <c r="G43" s="18">
+        <v>61</v>
+      </c>
+      <c r="C43" s="66" t="s">
+        <v>6</v>
+      </c>
+      <c r="D43" s="66"/>
+      <c r="E43" s="67"/>
+      <c r="F43" s="68">
+        <v>45392</v>
+      </c>
+      <c r="G43" s="69">
         <v>7</v>
       </c>
       <c r="H43" s="15"/>
@@ -9539,18 +9717,24 @@
       <c r="BK43" s="12"/>
       <c r="BL43" s="12"/>
     </row>
-    <row r="44" spans="1:65" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:65" s="1" customFormat="1" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A44" s="5"/>
       <c r="B44" s="19" t="s">
-        <v>58</v>
-      </c>
-      <c r="C44" s="15" t="s">
-        <v>27</v>
-      </c>
-      <c r="D44" s="15"/>
-      <c r="E44" s="16"/>
-      <c r="F44" s="17"/>
-      <c r="G44" s="18"/>
+        <v>65</v>
+      </c>
+      <c r="C44" s="66" t="s">
+        <v>6</v>
+      </c>
+      <c r="D44" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="E44" s="67"/>
+      <c r="F44" s="68">
+        <v>45393</v>
+      </c>
+      <c r="G44" s="69">
+        <v>6</v>
+      </c>
       <c r="H44" s="15"/>
       <c r="I44" s="12"/>
       <c r="J44" s="12"/>
@@ -9609,393 +9793,615 @@
       <c r="BK44" s="12"/>
       <c r="BL44" s="12"/>
     </row>
-    <row r="45" spans="1:65" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="5"/>
+    <row r="45" spans="1:65" s="1" customFormat="1" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A45" s="5" t="s">
+        <v>63</v>
+      </c>
       <c r="B45" s="19" t="s">
-        <v>57</v>
-      </c>
-      <c r="C45" s="15" t="s">
+        <v>64</v>
+      </c>
+      <c r="C45" s="66" t="s">
+        <v>7</v>
+      </c>
+      <c r="D45" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="E45" s="67"/>
+      <c r="F45" s="68">
+        <v>45399</v>
+      </c>
+      <c r="G45" s="69">
+        <v>1</v>
+      </c>
+      <c r="H45" s="15"/>
+      <c r="I45" s="12"/>
+      <c r="J45" s="12"/>
+      <c r="K45" s="12"/>
+      <c r="L45" s="12"/>
+      <c r="M45" s="12"/>
+      <c r="N45" s="12"/>
+      <c r="O45" s="12"/>
+      <c r="P45" s="12"/>
+      <c r="Q45" s="12"/>
+      <c r="R45" s="12"/>
+      <c r="S45" s="12"/>
+      <c r="T45" s="12"/>
+      <c r="U45" s="12"/>
+      <c r="V45" s="12"/>
+      <c r="W45" s="12"/>
+      <c r="X45" s="12"/>
+      <c r="Y45" s="12"/>
+      <c r="Z45" s="12"/>
+      <c r="AA45" s="12"/>
+      <c r="AB45" s="12"/>
+      <c r="AC45" s="12"/>
+      <c r="AD45" s="12"/>
+      <c r="AE45" s="12"/>
+      <c r="AF45" s="12"/>
+      <c r="AG45" s="12"/>
+      <c r="AH45" s="12"/>
+      <c r="AI45" s="12"/>
+      <c r="AJ45" s="12"/>
+      <c r="AK45" s="12"/>
+      <c r="AL45" s="12"/>
+      <c r="AM45" s="12"/>
+      <c r="AN45" s="12"/>
+      <c r="AO45" s="12"/>
+      <c r="AP45" s="12"/>
+      <c r="AQ45" s="12"/>
+      <c r="AR45" s="12"/>
+      <c r="AS45" s="12"/>
+      <c r="AT45" s="12"/>
+      <c r="AU45" s="12"/>
+      <c r="AV45" s="12"/>
+      <c r="AW45" s="12"/>
+      <c r="AX45" s="12"/>
+      <c r="AY45" s="12"/>
+      <c r="AZ45" s="12"/>
+      <c r="BA45" s="12"/>
+      <c r="BB45" s="12"/>
+      <c r="BC45" s="12"/>
+      <c r="BD45" s="12"/>
+      <c r="BE45" s="12"/>
+      <c r="BF45" s="12"/>
+      <c r="BG45" s="12"/>
+      <c r="BH45" s="12"/>
+      <c r="BI45" s="12"/>
+      <c r="BJ45" s="12"/>
+      <c r="BK45" s="12"/>
+      <c r="BL45" s="12"/>
+    </row>
+    <row r="46" spans="1:65" s="1" customFormat="1" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="5"/>
+      <c r="B46" s="19" t="s">
+        <v>59</v>
+      </c>
+      <c r="C46" s="66" t="s">
+        <v>6</v>
+      </c>
+      <c r="D46" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="E46" s="67"/>
+      <c r="F46" s="68">
+        <v>45400</v>
+      </c>
+      <c r="G46" s="69">
+        <v>7</v>
+      </c>
+      <c r="H46" s="15"/>
+      <c r="I46" s="12"/>
+      <c r="J46" s="12"/>
+      <c r="K46" s="12"/>
+      <c r="L46" s="12"/>
+      <c r="M46" s="12"/>
+      <c r="N46" s="12"/>
+      <c r="O46" s="12"/>
+      <c r="P46" s="12"/>
+      <c r="Q46" s="12"/>
+      <c r="R46" s="12"/>
+      <c r="S46" s="12"/>
+      <c r="T46" s="12"/>
+      <c r="U46" s="12"/>
+      <c r="V46" s="12"/>
+      <c r="W46" s="12"/>
+      <c r="X46" s="12"/>
+      <c r="Y46" s="12"/>
+      <c r="Z46" s="12"/>
+      <c r="AA46" s="12"/>
+      <c r="AB46" s="12"/>
+      <c r="AC46" s="12"/>
+      <c r="AD46" s="12"/>
+      <c r="AE46" s="12"/>
+      <c r="AF46" s="12"/>
+      <c r="AG46" s="12"/>
+      <c r="AH46" s="12"/>
+      <c r="AI46" s="12"/>
+      <c r="AJ46" s="12"/>
+      <c r="AK46" s="12"/>
+      <c r="AL46" s="12"/>
+      <c r="AM46" s="12"/>
+      <c r="AN46" s="12"/>
+      <c r="AO46" s="12"/>
+      <c r="AP46" s="12"/>
+      <c r="AQ46" s="12"/>
+      <c r="AR46" s="12"/>
+      <c r="AS46" s="12"/>
+      <c r="AT46" s="12"/>
+      <c r="AU46" s="12"/>
+      <c r="AV46" s="12"/>
+      <c r="AW46" s="12"/>
+      <c r="AX46" s="12"/>
+      <c r="AY46" s="12"/>
+      <c r="AZ46" s="12"/>
+      <c r="BA46" s="12"/>
+      <c r="BB46" s="12"/>
+      <c r="BC46" s="12"/>
+      <c r="BD46" s="12"/>
+      <c r="BE46" s="12"/>
+      <c r="BF46" s="12"/>
+      <c r="BG46" s="12"/>
+      <c r="BH46" s="12"/>
+      <c r="BI46" s="12"/>
+      <c r="BJ46" s="12"/>
+      <c r="BK46" s="12"/>
+      <c r="BL46" s="12"/>
+    </row>
+    <row r="47" spans="1:65" s="1" customFormat="1" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="5"/>
+      <c r="B47" s="19" t="s">
+        <v>54</v>
+      </c>
+      <c r="C47" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="D45" s="15"/>
-      <c r="E45" s="16"/>
-      <c r="F45" s="17"/>
-      <c r="G45" s="18"/>
-      <c r="H45" s="15"/>
-      <c r="I45" s="12" t="str">
-        <f t="shared" ref="I45:AN45" ca="1" si="29">IF(AND($C45="Doel",I$7&gt;=$F45,I$7&lt;=$F45+$G45-1),2,IF(AND($C45="Mijlpaal",I$7&gt;=$F45,I$7&lt;=$F45+$G45-1),1,""))</f>
-        <v/>
-      </c>
-      <c r="J45" s="12" t="str">
-        <f t="shared" ca="1" si="29"/>
-        <v/>
-      </c>
-      <c r="K45" s="12" t="str">
-        <f t="shared" ca="1" si="29"/>
-        <v/>
-      </c>
-      <c r="L45" s="12" t="str">
-        <f t="shared" ca="1" si="29"/>
-        <v/>
-      </c>
-      <c r="M45" s="12" t="str">
-        <f t="shared" ca="1" si="29"/>
-        <v/>
-      </c>
-      <c r="N45" s="12" t="str">
-        <f t="shared" ca="1" si="29"/>
-        <v/>
-      </c>
-      <c r="O45" s="12" t="str">
-        <f t="shared" ca="1" si="29"/>
-        <v/>
-      </c>
-      <c r="P45" s="12" t="str">
-        <f t="shared" ca="1" si="29"/>
-        <v/>
-      </c>
-      <c r="Q45" s="12" t="str">
-        <f t="shared" ca="1" si="29"/>
-        <v/>
-      </c>
-      <c r="R45" s="12" t="str">
-        <f t="shared" ca="1" si="29"/>
-        <v/>
-      </c>
-      <c r="S45" s="12" t="str">
-        <f t="shared" ca="1" si="29"/>
-        <v/>
-      </c>
-      <c r="T45" s="12" t="str">
-        <f t="shared" ca="1" si="29"/>
-        <v/>
-      </c>
-      <c r="U45" s="12" t="str">
-        <f t="shared" ca="1" si="29"/>
-        <v/>
-      </c>
-      <c r="V45" s="12" t="str">
-        <f t="shared" ca="1" si="29"/>
-        <v/>
-      </c>
-      <c r="W45" s="12" t="str">
-        <f t="shared" ca="1" si="29"/>
-        <v/>
-      </c>
-      <c r="X45" s="12" t="str">
-        <f t="shared" ca="1" si="29"/>
-        <v/>
-      </c>
-      <c r="Y45" s="12" t="str">
-        <f t="shared" ca="1" si="29"/>
-        <v/>
-      </c>
-      <c r="Z45" s="12" t="str">
-        <f t="shared" ca="1" si="29"/>
-        <v/>
-      </c>
-      <c r="AA45" s="12" t="str">
-        <f t="shared" ca="1" si="29"/>
-        <v/>
-      </c>
-      <c r="AB45" s="12" t="str">
-        <f t="shared" ca="1" si="29"/>
-        <v/>
-      </c>
-      <c r="AC45" s="12" t="str">
-        <f t="shared" ca="1" si="29"/>
-        <v/>
-      </c>
-      <c r="AD45" s="12" t="str">
-        <f t="shared" ca="1" si="29"/>
-        <v/>
-      </c>
-      <c r="AE45" s="12" t="str">
-        <f t="shared" ca="1" si="29"/>
-        <v/>
-      </c>
-      <c r="AF45" s="12" t="str">
-        <f t="shared" ca="1" si="29"/>
-        <v/>
-      </c>
-      <c r="AG45" s="12" t="str">
-        <f t="shared" ca="1" si="29"/>
-        <v/>
-      </c>
-      <c r="AH45" s="12" t="str">
-        <f t="shared" ca="1" si="29"/>
-        <v/>
-      </c>
-      <c r="AI45" s="12" t="str">
-        <f t="shared" ca="1" si="29"/>
-        <v/>
-      </c>
-      <c r="AJ45" s="12" t="str">
-        <f t="shared" ca="1" si="29"/>
-        <v/>
-      </c>
-      <c r="AK45" s="12" t="str">
-        <f t="shared" ca="1" si="29"/>
-        <v/>
-      </c>
-      <c r="AL45" s="12" t="str">
-        <f t="shared" ca="1" si="29"/>
-        <v/>
-      </c>
-      <c r="AM45" s="12" t="str">
-        <f t="shared" ca="1" si="29"/>
-        <v/>
-      </c>
-      <c r="AN45" s="12" t="str">
-        <f t="shared" ca="1" si="29"/>
-        <v/>
-      </c>
-      <c r="AO45" s="12" t="str">
-        <f t="shared" ref="AO45:BL45" ca="1" si="30">IF(AND($C45="Doel",AO$7&gt;=$F45,AO$7&lt;=$F45+$G45-1),2,IF(AND($C45="Mijlpaal",AO$7&gt;=$F45,AO$7&lt;=$F45+$G45-1),1,""))</f>
-        <v/>
-      </c>
-      <c r="AP45" s="12" t="str">
-        <f t="shared" ca="1" si="30"/>
-        <v/>
-      </c>
-      <c r="AQ45" s="12" t="str">
-        <f t="shared" ca="1" si="30"/>
-        <v/>
-      </c>
-      <c r="AR45" s="12" t="str">
-        <f t="shared" ca="1" si="30"/>
-        <v/>
-      </c>
-      <c r="AS45" s="12" t="str">
-        <f t="shared" ca="1" si="30"/>
-        <v/>
-      </c>
-      <c r="AT45" s="12" t="str">
-        <f t="shared" ca="1" si="30"/>
-        <v/>
-      </c>
-      <c r="AU45" s="12" t="str">
-        <f t="shared" ca="1" si="30"/>
-        <v/>
-      </c>
-      <c r="AV45" s="12" t="str">
-        <f t="shared" ca="1" si="30"/>
-        <v/>
-      </c>
-      <c r="AW45" s="12" t="str">
-        <f t="shared" ca="1" si="30"/>
-        <v/>
-      </c>
-      <c r="AX45" s="12" t="str">
-        <f t="shared" ca="1" si="30"/>
-        <v/>
-      </c>
-      <c r="AY45" s="12" t="str">
-        <f t="shared" ca="1" si="30"/>
-        <v/>
-      </c>
-      <c r="AZ45" s="12" t="str">
-        <f t="shared" ca="1" si="30"/>
-        <v/>
-      </c>
-      <c r="BA45" s="12" t="str">
-        <f t="shared" ca="1" si="30"/>
-        <v/>
-      </c>
-      <c r="BB45" s="12" t="str">
-        <f t="shared" ca="1" si="30"/>
-        <v/>
-      </c>
-      <c r="BC45" s="12" t="str">
-        <f t="shared" ca="1" si="30"/>
-        <v/>
-      </c>
-      <c r="BD45" s="12" t="str">
-        <f t="shared" ca="1" si="30"/>
-        <v/>
-      </c>
-      <c r="BE45" s="12" t="str">
-        <f t="shared" ca="1" si="30"/>
-        <v/>
-      </c>
-      <c r="BF45" s="12" t="str">
-        <f t="shared" ca="1" si="30"/>
-        <v/>
-      </c>
-      <c r="BG45" s="12" t="str">
-        <f t="shared" ca="1" si="30"/>
-        <v/>
-      </c>
-      <c r="BH45" s="12" t="str">
-        <f t="shared" ca="1" si="30"/>
-        <v/>
-      </c>
-      <c r="BI45" s="12" t="str">
-        <f t="shared" ca="1" si="30"/>
-        <v/>
-      </c>
-      <c r="BJ45" s="12" t="str">
-        <f t="shared" ca="1" si="30"/>
-        <v/>
-      </c>
-      <c r="BK45" s="12" t="str">
-        <f t="shared" ca="1" si="30"/>
-        <v/>
-      </c>
-      <c r="BL45" s="12" t="str">
-        <f t="shared" ca="1" si="30"/>
-        <v/>
-      </c>
-      <c r="BM45" s="42"/>
+      <c r="D47" s="15"/>
+      <c r="E47" s="16"/>
+      <c r="F47" s="17"/>
+      <c r="G47" s="18"/>
+      <c r="H47" s="15"/>
+      <c r="I47" s="12"/>
+      <c r="J47" s="12"/>
+      <c r="K47" s="12"/>
+      <c r="L47" s="12"/>
+      <c r="M47" s="12"/>
+      <c r="N47" s="12"/>
+      <c r="O47" s="12"/>
+      <c r="P47" s="12"/>
+      <c r="Q47" s="12"/>
+      <c r="R47" s="12"/>
+      <c r="S47" s="12"/>
+      <c r="T47" s="12"/>
+      <c r="U47" s="12"/>
+      <c r="V47" s="12"/>
+      <c r="W47" s="12"/>
+      <c r="X47" s="12"/>
+      <c r="Y47" s="12"/>
+      <c r="Z47" s="12"/>
+      <c r="AA47" s="12"/>
+      <c r="AB47" s="12"/>
+      <c r="AC47" s="12"/>
+      <c r="AD47" s="12"/>
+      <c r="AE47" s="12"/>
+      <c r="AF47" s="12"/>
+      <c r="AG47" s="12"/>
+      <c r="AH47" s="12"/>
+      <c r="AI47" s="12"/>
+      <c r="AJ47" s="12"/>
+      <c r="AK47" s="12"/>
+      <c r="AL47" s="12"/>
+      <c r="AM47" s="12"/>
+      <c r="AN47" s="12"/>
+      <c r="AO47" s="12"/>
+      <c r="AP47" s="12"/>
+      <c r="AQ47" s="12"/>
+      <c r="AR47" s="12"/>
+      <c r="AS47" s="12"/>
+      <c r="AT47" s="12"/>
+      <c r="AU47" s="12"/>
+      <c r="AV47" s="12"/>
+      <c r="AW47" s="12"/>
+      <c r="AX47" s="12"/>
+      <c r="AY47" s="12"/>
+      <c r="AZ47" s="12"/>
+      <c r="BA47" s="12"/>
+      <c r="BB47" s="12"/>
+      <c r="BC47" s="12"/>
+      <c r="BD47" s="12"/>
+      <c r="BE47" s="12"/>
+      <c r="BF47" s="12"/>
+      <c r="BG47" s="12"/>
+      <c r="BH47" s="12"/>
+      <c r="BI47" s="12"/>
+      <c r="BJ47" s="12"/>
+      <c r="BK47" s="12"/>
+      <c r="BL47" s="12"/>
     </row>
-    <row r="46" spans="1:65" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="5"/>
-      <c r="B46" s="61"/>
-      <c r="C46" s="15"/>
-      <c r="D46" s="15"/>
-      <c r="E46" s="16"/>
-      <c r="F46" s="17"/>
-      <c r="G46" s="18"/>
-      <c r="H46" s="15"/>
-      <c r="I46" s="68"/>
-      <c r="J46" s="68"/>
-      <c r="K46" s="68"/>
-      <c r="L46" s="68"/>
-      <c r="M46" s="68"/>
-      <c r="N46" s="68"/>
-      <c r="O46" s="68"/>
-      <c r="P46" s="68"/>
-      <c r="Q46" s="68"/>
-      <c r="R46" s="68"/>
-      <c r="S46" s="68"/>
-      <c r="T46" s="68"/>
-      <c r="U46" s="68"/>
-      <c r="V46" s="68"/>
-      <c r="W46" s="68"/>
-      <c r="X46" s="68"/>
-      <c r="Y46" s="68"/>
-      <c r="Z46" s="68"/>
-      <c r="AA46" s="68"/>
-      <c r="AB46" s="68"/>
-      <c r="AC46" s="68"/>
-      <c r="AD46" s="68"/>
-      <c r="AE46" s="68"/>
-      <c r="AF46" s="68"/>
-      <c r="AG46" s="68"/>
-      <c r="AH46" s="68"/>
-      <c r="AI46" s="68"/>
-      <c r="AJ46" s="68"/>
-      <c r="AK46" s="68"/>
-      <c r="AL46" s="68"/>
-      <c r="AM46" s="68"/>
-      <c r="AN46" s="68"/>
-      <c r="AO46" s="68"/>
-      <c r="AP46" s="68"/>
-      <c r="AQ46" s="68"/>
-      <c r="AR46" s="68"/>
-      <c r="AS46" s="68"/>
-      <c r="AT46" s="68"/>
-      <c r="AU46" s="68"/>
-      <c r="AV46" s="68"/>
-      <c r="AW46" s="68"/>
-      <c r="AX46" s="68"/>
-      <c r="AY46" s="68"/>
-      <c r="AZ46" s="68"/>
-      <c r="BA46" s="68"/>
-      <c r="BB46" s="68"/>
-      <c r="BC46" s="68"/>
-      <c r="BD46" s="68"/>
-      <c r="BE46" s="68"/>
-      <c r="BF46" s="68"/>
-      <c r="BG46" s="68"/>
-      <c r="BH46" s="68"/>
-      <c r="BI46" s="68"/>
-      <c r="BJ46" s="68"/>
-      <c r="BK46" s="68"/>
-      <c r="BL46" s="68"/>
-      <c r="BM46" s="69"/>
+    <row r="48" spans="1:65" s="1" customFormat="1" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A48" s="5"/>
+      <c r="B48" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="C48" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="D48" s="15"/>
+      <c r="E48" s="16"/>
+      <c r="F48" s="17"/>
+      <c r="G48" s="18"/>
+      <c r="H48" s="15"/>
+      <c r="I48" s="12" t="str">
+        <f t="shared" ref="I48:AN48" ca="1" si="31">IF(AND($C48="Doel",I$7&gt;=$F48,I$7&lt;=$F48+$G48-1),2,IF(AND($C48="Mijlpaal",I$7&gt;=$F48,I$7&lt;=$F48+$G48-1),1,""))</f>
+        <v/>
+      </c>
+      <c r="J48" s="12" t="str">
+        <f t="shared" ca="1" si="31"/>
+        <v/>
+      </c>
+      <c r="K48" s="12" t="str">
+        <f t="shared" ca="1" si="31"/>
+        <v/>
+      </c>
+      <c r="L48" s="12" t="str">
+        <f t="shared" ca="1" si="31"/>
+        <v/>
+      </c>
+      <c r="M48" s="12" t="str">
+        <f t="shared" ca="1" si="31"/>
+        <v/>
+      </c>
+      <c r="N48" s="12" t="str">
+        <f t="shared" ca="1" si="31"/>
+        <v/>
+      </c>
+      <c r="O48" s="12" t="str">
+        <f t="shared" ca="1" si="31"/>
+        <v/>
+      </c>
+      <c r="P48" s="12" t="str">
+        <f t="shared" ca="1" si="31"/>
+        <v/>
+      </c>
+      <c r="Q48" s="12" t="str">
+        <f t="shared" ca="1" si="31"/>
+        <v/>
+      </c>
+      <c r="R48" s="12" t="str">
+        <f t="shared" ca="1" si="31"/>
+        <v/>
+      </c>
+      <c r="S48" s="12" t="str">
+        <f t="shared" ca="1" si="31"/>
+        <v/>
+      </c>
+      <c r="T48" s="12" t="str">
+        <f t="shared" ca="1" si="31"/>
+        <v/>
+      </c>
+      <c r="U48" s="12" t="str">
+        <f t="shared" ca="1" si="31"/>
+        <v/>
+      </c>
+      <c r="V48" s="12" t="str">
+        <f t="shared" ca="1" si="31"/>
+        <v/>
+      </c>
+      <c r="W48" s="12" t="str">
+        <f t="shared" ca="1" si="31"/>
+        <v/>
+      </c>
+      <c r="X48" s="12" t="str">
+        <f t="shared" ca="1" si="31"/>
+        <v/>
+      </c>
+      <c r="Y48" s="12" t="str">
+        <f t="shared" ca="1" si="31"/>
+        <v/>
+      </c>
+      <c r="Z48" s="12" t="str">
+        <f t="shared" ca="1" si="31"/>
+        <v/>
+      </c>
+      <c r="AA48" s="12" t="str">
+        <f t="shared" ca="1" si="31"/>
+        <v/>
+      </c>
+      <c r="AB48" s="12" t="str">
+        <f t="shared" ca="1" si="31"/>
+        <v/>
+      </c>
+      <c r="AC48" s="12" t="str">
+        <f t="shared" ca="1" si="31"/>
+        <v/>
+      </c>
+      <c r="AD48" s="12" t="str">
+        <f t="shared" ca="1" si="31"/>
+        <v/>
+      </c>
+      <c r="AE48" s="12" t="str">
+        <f t="shared" ca="1" si="31"/>
+        <v/>
+      </c>
+      <c r="AF48" s="12" t="str">
+        <f t="shared" ca="1" si="31"/>
+        <v/>
+      </c>
+      <c r="AG48" s="12" t="str">
+        <f t="shared" ca="1" si="31"/>
+        <v/>
+      </c>
+      <c r="AH48" s="12" t="str">
+        <f t="shared" ca="1" si="31"/>
+        <v/>
+      </c>
+      <c r="AI48" s="12" t="str">
+        <f t="shared" ca="1" si="31"/>
+        <v/>
+      </c>
+      <c r="AJ48" s="12" t="str">
+        <f t="shared" ca="1" si="31"/>
+        <v/>
+      </c>
+      <c r="AK48" s="12" t="str">
+        <f t="shared" ca="1" si="31"/>
+        <v/>
+      </c>
+      <c r="AL48" s="12" t="str">
+        <f t="shared" ca="1" si="31"/>
+        <v/>
+      </c>
+      <c r="AM48" s="12" t="str">
+        <f t="shared" ca="1" si="31"/>
+        <v/>
+      </c>
+      <c r="AN48" s="12" t="str">
+        <f t="shared" ca="1" si="31"/>
+        <v/>
+      </c>
+      <c r="AO48" s="12" t="str">
+        <f t="shared" ref="AO48:BL48" ca="1" si="32">IF(AND($C48="Doel",AO$7&gt;=$F48,AO$7&lt;=$F48+$G48-1),2,IF(AND($C48="Mijlpaal",AO$7&gt;=$F48,AO$7&lt;=$F48+$G48-1),1,""))</f>
+        <v/>
+      </c>
+      <c r="AP48" s="12" t="str">
+        <f t="shared" ca="1" si="32"/>
+        <v/>
+      </c>
+      <c r="AQ48" s="12" t="str">
+        <f t="shared" ca="1" si="32"/>
+        <v/>
+      </c>
+      <c r="AR48" s="12" t="str">
+        <f t="shared" ca="1" si="32"/>
+        <v/>
+      </c>
+      <c r="AS48" s="12" t="str">
+        <f t="shared" ca="1" si="32"/>
+        <v/>
+      </c>
+      <c r="AT48" s="12" t="str">
+        <f t="shared" ca="1" si="32"/>
+        <v/>
+      </c>
+      <c r="AU48" s="12" t="str">
+        <f t="shared" ca="1" si="32"/>
+        <v/>
+      </c>
+      <c r="AV48" s="12" t="str">
+        <f t="shared" ca="1" si="32"/>
+        <v/>
+      </c>
+      <c r="AW48" s="12" t="str">
+        <f t="shared" ca="1" si="32"/>
+        <v/>
+      </c>
+      <c r="AX48" s="12" t="str">
+        <f t="shared" ca="1" si="32"/>
+        <v/>
+      </c>
+      <c r="AY48" s="12" t="str">
+        <f t="shared" ca="1" si="32"/>
+        <v/>
+      </c>
+      <c r="AZ48" s="12" t="str">
+        <f t="shared" ca="1" si="32"/>
+        <v/>
+      </c>
+      <c r="BA48" s="12" t="str">
+        <f t="shared" ca="1" si="32"/>
+        <v/>
+      </c>
+      <c r="BB48" s="12" t="str">
+        <f t="shared" ca="1" si="32"/>
+        <v/>
+      </c>
+      <c r="BC48" s="12" t="str">
+        <f t="shared" ca="1" si="32"/>
+        <v/>
+      </c>
+      <c r="BD48" s="12" t="str">
+        <f t="shared" ca="1" si="32"/>
+        <v/>
+      </c>
+      <c r="BE48" s="12" t="str">
+        <f t="shared" ca="1" si="32"/>
+        <v/>
+      </c>
+      <c r="BF48" s="12" t="str">
+        <f t="shared" ca="1" si="32"/>
+        <v/>
+      </c>
+      <c r="BG48" s="12" t="str">
+        <f t="shared" ca="1" si="32"/>
+        <v/>
+      </c>
+      <c r="BH48" s="12" t="str">
+        <f t="shared" ca="1" si="32"/>
+        <v/>
+      </c>
+      <c r="BI48" s="12" t="str">
+        <f t="shared" ca="1" si="32"/>
+        <v/>
+      </c>
+      <c r="BJ48" s="12" t="str">
+        <f t="shared" ca="1" si="32"/>
+        <v/>
+      </c>
+      <c r="BK48" s="12" t="str">
+        <f t="shared" ca="1" si="32"/>
+        <v/>
+      </c>
+      <c r="BL48" s="12" t="str">
+        <f t="shared" ca="1" si="32"/>
+        <v/>
+      </c>
+      <c r="BM48" s="42"/>
     </row>
-    <row r="47" spans="1:65" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="6"/>
-      <c r="B47" s="50" t="s">
+    <row r="49" spans="1:64" s="1" customFormat="1" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A49" s="5"/>
+      <c r="B49" s="61"/>
+      <c r="C49" s="15"/>
+      <c r="D49" s="15"/>
+      <c r="E49" s="16"/>
+      <c r="F49" s="17"/>
+      <c r="G49" s="18"/>
+      <c r="H49" s="15"/>
+      <c r="I49" s="40"/>
+      <c r="J49" s="40"/>
+      <c r="K49" s="40"/>
+      <c r="L49" s="40"/>
+      <c r="M49" s="40"/>
+      <c r="N49" s="40"/>
+      <c r="O49" s="40"/>
+      <c r="P49" s="40"/>
+      <c r="Q49" s="40"/>
+      <c r="R49" s="40"/>
+      <c r="S49" s="40"/>
+      <c r="T49" s="40"/>
+      <c r="U49" s="40"/>
+      <c r="V49" s="40"/>
+      <c r="W49" s="40"/>
+      <c r="X49" s="40"/>
+      <c r="Y49" s="40"/>
+      <c r="Z49" s="40"/>
+      <c r="AA49" s="40"/>
+      <c r="AB49" s="40"/>
+      <c r="AC49" s="40"/>
+      <c r="AD49" s="40"/>
+      <c r="AE49" s="40"/>
+      <c r="AF49" s="40"/>
+      <c r="AG49" s="40"/>
+      <c r="AH49" s="40"/>
+      <c r="AI49" s="40"/>
+      <c r="AJ49" s="40"/>
+      <c r="AK49" s="40"/>
+      <c r="AL49" s="40"/>
+      <c r="AM49" s="40"/>
+      <c r="AN49" s="40"/>
+      <c r="AO49" s="40"/>
+      <c r="AP49" s="40"/>
+      <c r="AQ49" s="40"/>
+      <c r="AR49" s="40"/>
+      <c r="AS49" s="40"/>
+      <c r="AT49" s="40"/>
+      <c r="AU49" s="40"/>
+      <c r="AV49" s="40"/>
+      <c r="AW49" s="40"/>
+      <c r="AX49" s="40"/>
+      <c r="AY49" s="40"/>
+      <c r="AZ49" s="40"/>
+      <c r="BA49" s="40"/>
+      <c r="BB49" s="40"/>
+      <c r="BC49" s="40"/>
+      <c r="BD49" s="40"/>
+      <c r="BE49" s="40"/>
+      <c r="BF49" s="40"/>
+      <c r="BG49" s="40"/>
+      <c r="BH49" s="40"/>
+      <c r="BI49" s="40"/>
+      <c r="BJ49" s="40"/>
+      <c r="BK49" s="40"/>
+      <c r="BL49" s="40"/>
+    </row>
+    <row r="50" spans="1:64" s="1" customFormat="1" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A50" s="6"/>
+      <c r="B50" s="50" t="s">
         <v>3</v>
       </c>
-      <c r="C47" s="15"/>
-      <c r="D47" s="15"/>
-      <c r="E47" s="28"/>
-      <c r="F47" s="38"/>
-      <c r="G47" s="39"/>
-      <c r="H47" s="15"/>
-      <c r="I47" s="40"/>
-      <c r="J47" s="40"/>
-      <c r="K47" s="40"/>
-      <c r="L47" s="40"/>
-      <c r="M47" s="40"/>
-      <c r="N47" s="40"/>
-      <c r="O47" s="40"/>
-      <c r="P47" s="40"/>
-      <c r="Q47" s="40"/>
-      <c r="R47" s="40"/>
-      <c r="S47" s="40"/>
-      <c r="T47" s="40"/>
-      <c r="U47" s="40"/>
-      <c r="V47" s="40"/>
-      <c r="W47" s="40"/>
-      <c r="X47" s="40"/>
-      <c r="Y47" s="40"/>
-      <c r="Z47" s="40"/>
-      <c r="AA47" s="40"/>
-      <c r="AB47" s="40"/>
-      <c r="AC47" s="40"/>
-      <c r="AD47" s="40"/>
-      <c r="AE47" s="40"/>
-      <c r="AF47" s="40"/>
-      <c r="AG47" s="40"/>
-      <c r="AH47" s="40"/>
-      <c r="AI47" s="40"/>
-      <c r="AJ47" s="40"/>
-      <c r="AK47" s="40"/>
-      <c r="AL47" s="40"/>
-      <c r="AM47" s="40"/>
-      <c r="AN47" s="40"/>
-      <c r="AO47" s="40"/>
-      <c r="AP47" s="40"/>
-      <c r="AQ47" s="40"/>
-      <c r="AR47" s="40"/>
-      <c r="AS47" s="40"/>
-      <c r="AT47" s="40"/>
-      <c r="AU47" s="40"/>
-      <c r="AV47" s="40"/>
-      <c r="AW47" s="40"/>
-      <c r="AX47" s="40"/>
-      <c r="AY47" s="40"/>
-      <c r="AZ47" s="40"/>
-      <c r="BA47" s="40"/>
-      <c r="BB47" s="40"/>
-      <c r="BC47" s="40"/>
-      <c r="BD47" s="40"/>
-      <c r="BE47" s="40"/>
-      <c r="BF47" s="40"/>
-      <c r="BG47" s="40"/>
-      <c r="BH47" s="40"/>
-      <c r="BI47" s="40"/>
-      <c r="BJ47" s="40"/>
-      <c r="BK47" s="40"/>
-      <c r="BL47" s="40"/>
+      <c r="C50" s="15"/>
+      <c r="D50" s="15"/>
+      <c r="E50" s="28"/>
+      <c r="F50" s="38"/>
+      <c r="G50" s="39"/>
+      <c r="H50" s="15"/>
+      <c r="I50" s="40"/>
+      <c r="J50" s="40"/>
+      <c r="K50" s="40"/>
+      <c r="L50" s="40"/>
+      <c r="M50" s="40"/>
+      <c r="N50" s="40"/>
+      <c r="O50" s="40"/>
+      <c r="P50" s="40"/>
+      <c r="Q50" s="40"/>
+      <c r="R50" s="40"/>
+      <c r="S50" s="40"/>
+      <c r="T50" s="40"/>
+      <c r="U50" s="40"/>
+      <c r="V50" s="40"/>
+      <c r="W50" s="40"/>
+      <c r="X50" s="40"/>
+      <c r="Y50" s="40"/>
+      <c r="Z50" s="40"/>
+      <c r="AA50" s="40"/>
+      <c r="AB50" s="40"/>
+      <c r="AC50" s="40"/>
+      <c r="AD50" s="40"/>
+      <c r="AE50" s="40"/>
+      <c r="AF50" s="40"/>
+      <c r="AG50" s="40"/>
+      <c r="AH50" s="40"/>
+      <c r="AI50" s="40"/>
+      <c r="AJ50" s="40"/>
+      <c r="AK50" s="40"/>
+      <c r="AL50" s="40"/>
+      <c r="AM50" s="40"/>
+      <c r="AN50" s="40"/>
+      <c r="AO50" s="40"/>
+      <c r="AP50" s="40"/>
+      <c r="AQ50" s="40"/>
+      <c r="AR50" s="40"/>
+      <c r="AS50" s="40"/>
+      <c r="AT50" s="40"/>
+      <c r="AU50" s="40"/>
+      <c r="AV50" s="40"/>
+      <c r="AW50" s="40"/>
+      <c r="AX50" s="40"/>
+      <c r="AY50" s="40"/>
+      <c r="AZ50" s="40"/>
+      <c r="BA50" s="40"/>
+      <c r="BB50" s="40"/>
+      <c r="BC50" s="40"/>
+      <c r="BD50" s="40"/>
+      <c r="BE50" s="40"/>
+      <c r="BF50" s="40"/>
+      <c r="BG50" s="40"/>
+      <c r="BH50" s="40"/>
+      <c r="BI50" s="40"/>
+      <c r="BJ50" s="40"/>
+      <c r="BK50" s="40"/>
+      <c r="BL50" s="40"/>
     </row>
-    <row r="48" spans="1:65" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B48" s="62" t="s">
-        <v>56</v>
-      </c>
-      <c r="C48" s="63"/>
-      <c r="D48" s="65"/>
-      <c r="E48" s="66"/>
-      <c r="F48" s="64"/>
-      <c r="G48" s="67"/>
-      <c r="H48" s="3"/>
+    <row r="51" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B51" s="62" t="s">
+        <v>52</v>
+      </c>
+      <c r="C51" s="40"/>
+      <c r="D51" s="64"/>
+      <c r="F51" s="63"/>
+      <c r="G51" s="65"/>
+      <c r="H51" s="3"/>
     </row>
-    <row r="49" spans="4:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D49" s="4"/>
+    <row r="52" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D52" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="8">
@@ -10008,8 +10414,8 @@
     <mergeCell ref="N4:Q4"/>
     <mergeCell ref="S4:X4"/>
   </mergeCells>
-  <conditionalFormatting sqref="E9:E48">
-    <cfRule type="dataBar" priority="20">
+  <conditionalFormatting sqref="E9:E51">
+    <cfRule type="dataBar" priority="25">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -10022,97 +10428,131 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I7:BL17 P18:BL22 I18:N22 I23:BL47">
-    <cfRule type="expression" dxfId="26" priority="16">
+  <conditionalFormatting sqref="I7:BL17 P18:BL22 I18:N22 I23:BL50">
+    <cfRule type="expression" dxfId="36" priority="21">
       <formula>AND(TODAY()&gt;=I$7,TODAY()&lt;J$7)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I6:AM6">
-    <cfRule type="expression" dxfId="25" priority="19">
+    <cfRule type="expression" dxfId="35" priority="24">
       <formula>I$7&lt;=EOMONTH($I$7,0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J6:BL6">
-    <cfRule type="expression" dxfId="24" priority="18">
+    <cfRule type="expression" dxfId="34" priority="23">
       <formula>AND(J$7&lt;=EOMONTH($I$7,2),J$7&gt;EOMONTH($I$7,0),J$7&gt;EOMONTH($I$7,1))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I6:BL6">
-    <cfRule type="expression" dxfId="23" priority="17">
+    <cfRule type="expression" dxfId="33" priority="22">
       <formula>AND(I$7&lt;=EOMONTH($I$7,1),I$7&gt;EOMONTH($I$7,0))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I10:BL17 P21:BL22 P18:BL19 I18:N22 I23:BL46">
-    <cfRule type="expression" dxfId="22" priority="22" stopIfTrue="1">
+  <conditionalFormatting sqref="I10:BL17 P21:BL22 P18:BL19 I18:N22 I23:BL49">
+    <cfRule type="expression" dxfId="32" priority="27" stopIfTrue="1">
       <formula>AND($C10="Laag risico",I$7&gt;=$F10,I$7&lt;=$F10+$G10-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="21" priority="23" stopIfTrue="1">
+    <cfRule type="expression" dxfId="31" priority="28" stopIfTrue="1">
       <formula>AND($C10="Hoog risico",I$7&gt;=$F10,I$7&lt;=$F10+$G10-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="20" priority="24" stopIfTrue="1">
+    <cfRule type="expression" dxfId="30" priority="29" stopIfTrue="1">
       <formula>AND($C10="Op schema",I$7&gt;=$F10,I$7&lt;=$F10+$G10-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="19" priority="25" stopIfTrue="1">
+    <cfRule type="expression" dxfId="29" priority="30" stopIfTrue="1">
       <formula>AND($C10="Gemiddeld risico",I$7&gt;=$F10,I$7&lt;=$F10+$G10-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="18" priority="26" stopIfTrue="1">
+    <cfRule type="expression" dxfId="28" priority="31" stopIfTrue="1">
       <formula>AND(LEN($C10)=0,I$7&gt;=$F10,I$7&lt;=$F10+$G10-1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P20:BL20">
-    <cfRule type="expression" dxfId="17" priority="35" stopIfTrue="1">
+    <cfRule type="expression" dxfId="27" priority="40" stopIfTrue="1">
       <formula>AND($C20="Laag risico",P$7&gt;=#REF!,P$7&lt;=#REF!+$G20-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="16" priority="36" stopIfTrue="1">
+    <cfRule type="expression" dxfId="26" priority="41" stopIfTrue="1">
       <formula>AND($C20="Hoog risico",P$7&gt;=#REF!,P$7&lt;=#REF!+$G20-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="15" priority="37" stopIfTrue="1">
+    <cfRule type="expression" dxfId="25" priority="42" stopIfTrue="1">
       <formula>AND($C20="Op schema",P$7&gt;=#REF!,P$7&lt;=#REF!+$G20-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="14" priority="38" stopIfTrue="1">
+    <cfRule type="expression" dxfId="24" priority="43" stopIfTrue="1">
       <formula>AND($C20="Gemiddeld risico",P$7&gt;=#REF!,P$7&lt;=#REF!+$G20-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="13" priority="39" stopIfTrue="1">
+    <cfRule type="expression" dxfId="23" priority="44" stopIfTrue="1">
       <formula>AND(LEN($C20)=0,P$7&gt;=#REF!,P$7&lt;=#REF!+$G20-1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P20:BL20">
-    <cfRule type="expression" dxfId="12" priority="11" stopIfTrue="1">
+    <cfRule type="expression" dxfId="22" priority="16" stopIfTrue="1">
       <formula>AND($C20="Laag risico",P$7&gt;=$F20,P$7&lt;=$F20+$G20-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="11" priority="12" stopIfTrue="1">
+    <cfRule type="expression" dxfId="21" priority="17" stopIfTrue="1">
       <formula>AND($C20="Hoog risico",P$7&gt;=$F20,P$7&lt;=$F20+$G20-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="10" priority="13" stopIfTrue="1">
+    <cfRule type="expression" dxfId="20" priority="18" stopIfTrue="1">
       <formula>AND($C20="Op schema",P$7&gt;=$F20,P$7&lt;=$F20+$G20-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="9" priority="14" stopIfTrue="1">
+    <cfRule type="expression" dxfId="19" priority="19" stopIfTrue="1">
       <formula>AND($C20="Gemiddeld risico",P$7&gt;=$F20,P$7&lt;=$F20+$G20-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="8" priority="15" stopIfTrue="1">
+    <cfRule type="expression" dxfId="18" priority="20" stopIfTrue="1">
       <formula>AND(LEN($C20)=0,P$7&gt;=$F20,P$7&lt;=$F20+$G20-1)</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="AF41:AO41">
+    <cfRule type="expression" dxfId="17" priority="257" stopIfTrue="1">
+      <formula>AND(#REF!="Laag risico",AF$7&gt;=#REF!,AF$7&lt;=#REF!+#REF!-1)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="16" priority="258" stopIfTrue="1">
+      <formula>AND(#REF!="Hoog risico",AF$7&gt;=#REF!,AF$7&lt;=#REF!+#REF!-1)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="15" priority="259" stopIfTrue="1">
+      <formula>AND(#REF!="Op schema",AF$7&gt;=#REF!,AF$7&lt;=#REF!+#REF!-1)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="14" priority="260" stopIfTrue="1">
+      <formula>AND(#REF!="Gemiddeld risico",AF$7&gt;=#REF!,AF$7&lt;=#REF!+#REF!-1)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="13" priority="261" stopIfTrue="1">
+      <formula>AND(LEN(#REF!)=0,AF$7&gt;=#REF!,AF$7&lt;=#REF!+#REF!-1)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AF40:AO40">
+    <cfRule type="expression" dxfId="12" priority="271" stopIfTrue="1">
+      <formula>AND(#REF!="Laag risico",AF$7&gt;=#REF!,AF$7&lt;=#REF!+#REF!-1)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="11" priority="272" stopIfTrue="1">
+      <formula>AND(#REF!="Hoog risico",AF$7&gt;=#REF!,AF$7&lt;=#REF!+#REF!-1)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="10" priority="273" stopIfTrue="1">
+      <formula>AND(#REF!="Op schema",AF$7&gt;=#REF!,AF$7&lt;=#REF!+#REF!-1)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="9" priority="274" stopIfTrue="1">
+      <formula>AND(#REF!="Gemiddeld risico",AF$7&gt;=#REF!,AF$7&lt;=#REF!+#REF!-1)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="8" priority="275" stopIfTrue="1">
+      <formula>AND(LEN(#REF!)=0,AF$7&gt;=#REF!,AF$7&lt;=#REF!+#REF!-1)</formula>
+    </cfRule>
+  </conditionalFormatting>
   <dataValidations count="13">
-    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" promptTitle="Scrolverhoging" prompt="Als u dit getal wijzigt, scrolt u door de weergave van het Gantt-diagram." sqref="C7">
+    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" promptTitle="Scrolverhoging" prompt="Als u dit getal wijzigt, scrolt u door de weergave van het Gantt-diagram." sqref="C7" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>0</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C10 C12:C46">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C10 C12:C49" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>"Doel,Mijlpaal,Op schema, Laag risico, Gemiddeld risico, Hoog risico"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" sqref="C11">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" sqref="C11" xr:uid="{00000000-0002-0000-0000-000002000000}">
       <formula1>"Doel,Mijlpaal,Op schema, Laag risico, Gemiddeld risico, Hoog risico"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Een Gantt-diagram maken" prompt="Voer de titel van dit project in cel B2 in. _x000a_Informatie over het gebruik van dit werkblad, met in het werkblad Info over instructies voor schermlezers en de auteur van deze werkmap._x000a_Ga verder in kolom A om meer instructies te horen." sqref="A2"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Voer de bedrijfsnaam in cel B4 in._x000a_De legenda staat in cellen I4 tot en met AC4. Het label Legenda staat in cel G4." sqref="A4"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Voer de naam van de projectleider in cel B5 in. Voer de begindatum van het project in cel C6 in of zoek de kleinste datumwaarde met de voorbeeldformule in tabel Gantt-gegevens._x000a_Begindatum van project: het label staat in cel B6." sqref="A5"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Cel C7 bevat een scrolverhoging. _x000a_De maanden voor de datums in rij 7 worden weergegeven vanaf cel I6 tot en met cel BL6._x000a_Wijzig deze cellen. Ze worden automatisch bijgewerkt op basis van de begindatum van het project in cel F6." sqref="A6"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Cellen I9 tot en met BL9 bevatten het dagnummer van de maand voor de maand in het celblok boven elke datumcel en worden automatisch berekend._x000a_Wijzig deze cellen niet._x000a_" sqref="A7"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Een schuifbalk staat in cellen I8 tot en met BL8. _x000a_Als u in de tijdlijn vooruit of achteruit wilt gaan, voert u een waarde van 0 of hoger in cel C7 in._x000a_Met de waarde 0 gaat u naar het begin van het diagram." sqref="A8"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="De rij bevat headers voor de projectplanning. Cellen B9 tot en met G9 bevatten planningsinfo. I9 tot en met BL9 bevatten de eerste letter van elke weekdag voor de datum boven de kop._x000a_Elk diagram van een projecttijdlijn wordt automatisch gegenereerd." sqref="A9"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Voer projectinfo in vanaf cel B11 tot en met cel G11. _x000a_Voer de beschrijving van de mijlpaal in, selecteer een categorie, wijs iemand de taak toe en voer de voortgang, de begindatum en het aantal dagen voor de taak in om het diagram te maken._x000a_" sqref="A11"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Deze rij markeert het einde van de Gantt-mijlpaalgegevens. Voer NIETS in deze rij in. _x000a_Als u meer items wilt toevoegen, voegt u nieuwe rijen boven deze in._x000a_" sqref="A47"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Dit is een lege rij" sqref="A45:A46"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Een Gantt-diagram maken" prompt="Voer de titel van dit project in cel B2 in. _x000a_Informatie over het gebruik van dit werkblad, met in het werkblad Info over instructies voor schermlezers en de auteur van deze werkmap._x000a_Ga verder in kolom A om meer instructies te horen." sqref="A2" xr:uid="{00000000-0002-0000-0000-000003000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Voer de bedrijfsnaam in cel B4 in._x000a_De legenda staat in cellen I4 tot en met AC4. Het label Legenda staat in cel G4." sqref="A4" xr:uid="{00000000-0002-0000-0000-000004000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Voer de naam van de projectleider in cel B5 in. Voer de begindatum van het project in cel C6 in of zoek de kleinste datumwaarde met de voorbeeldformule in tabel Gantt-gegevens._x000a_Begindatum van project: het label staat in cel B6." sqref="A5" xr:uid="{00000000-0002-0000-0000-000005000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Cel C7 bevat een scrolverhoging. _x000a_De maanden voor de datums in rij 7 worden weergegeven vanaf cel I6 tot en met cel BL6._x000a_Wijzig deze cellen. Ze worden automatisch bijgewerkt op basis van de begindatum van het project in cel F6." sqref="A6" xr:uid="{00000000-0002-0000-0000-000006000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Cellen I9 tot en met BL9 bevatten het dagnummer van de maand voor de maand in het celblok boven elke datumcel en worden automatisch berekend._x000a_Wijzig deze cellen niet._x000a_" sqref="A7" xr:uid="{00000000-0002-0000-0000-000007000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Een schuifbalk staat in cellen I8 tot en met BL8. _x000a_Als u in de tijdlijn vooruit of achteruit wilt gaan, voert u een waarde van 0 of hoger in cel C7 in._x000a_Met de waarde 0 gaat u naar het begin van het diagram." sqref="A8" xr:uid="{00000000-0002-0000-0000-000008000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="De rij bevat headers voor de projectplanning. Cellen B9 tot en met G9 bevatten planningsinfo. I9 tot en met BL9 bevatten de eerste letter van elke weekdag voor de datum boven de kop._x000a_Elk diagram van een projecttijdlijn wordt automatisch gegenereerd." sqref="A9" xr:uid="{00000000-0002-0000-0000-000009000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Voer projectinfo in vanaf cel B11 tot en met cel G11. _x000a_Voer de beschrijving van de mijlpaal in, selecteer een categorie, wijs iemand de taak toe en voer de voortgang, de begindatum en het aantal dagen voor de taak in om het diagram te maken._x000a_" sqref="A11" xr:uid="{00000000-0002-0000-0000-00000A000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Deze rij markeert het einde van de Gantt-mijlpaalgegevens. Voer NIETS in deze rij in. _x000a_Als u meer items wilt toevoegen, voegt u nieuwe rijen boven deze in._x000a_" sqref="A50" xr:uid="{00000000-0002-0000-0000-00000B000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Dit is een lege rij" sqref="A48:A49" xr:uid="{00000000-0002-0000-0000-00000C000000}"/>
   </dataValidations>
   <pageMargins left="0.5" right="0.5" top="0.5" bottom="0.5" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="95" fitToHeight="0" orientation="portrait" r:id="rId1"/>
@@ -10136,15 +10576,15 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>8</xdr:col>
-                    <xdr:colOff>28575</xdr:colOff>
+                    <xdr:colOff>30480</xdr:colOff>
                     <xdr:row>7</xdr:row>
-                    <xdr:rowOff>57150</xdr:rowOff>
+                    <xdr:rowOff>60960</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>63</xdr:col>
                     <xdr:colOff>228600</xdr:colOff>
                     <xdr:row>7</xdr:row>
-                    <xdr:rowOff>238125</xdr:rowOff>
+                    <xdr:rowOff>236220</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -10173,10 +10613,10 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>E9:E48</xm:sqref>
+          <xm:sqref>E9:E51</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="27" id="{A1EFF969-3CBB-4DB2-A4C9-47B01FE32C86}">
+          <x14:cfRule type="iconSet" priority="32" id="{A1EFF969-3CBB-4DB2-A4C9-47B01FE32C86}">
             <x14:iconSet iconSet="3Stars" showValue="0" custom="1">
               <x14:cfvo type="percent">
                 <xm:f>0</xm:f>
@@ -10192,10 +10632,10 @@
               <x14:cfIcon iconSet="3Signs" iconId="0"/>
             </x14:iconSet>
           </x14:cfRule>
-          <xm:sqref>I47:BL47</xm:sqref>
+          <xm:sqref>I50:BL50</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="69" id="{39412BF5-D1E8-4731-95F6-6B0C252D35F8}">
+          <x14:cfRule type="iconSet" priority="276" id="{39412BF5-D1E8-4731-95F6-6B0C252D35F8}">
             <x14:iconSet iconSet="3Stars" showValue="0" custom="1">
               <x14:cfvo type="percent">
                 <xm:f>0</xm:f>
@@ -10211,7 +10651,7 @@
               <x14:cfIcon iconSet="3Signs" iconId="0"/>
             </x14:iconSet>
           </x14:cfRule>
-          <xm:sqref>I10:BL17 I23:BL46 P18:BL22 I18:N22</xm:sqref>
+          <xm:sqref>I10:BL17 P18:BL22 I18:N22 I23:BL49</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>

</xml_diff>